<commit_message>
including cleaned time table in preprocessing script
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -819,7 +819,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr"/>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="AA22" t="inlineStr">
         <is>
-          <t>Mz3</t>
+          <t>Mz</t>
         </is>
       </c>
       <c r="AB22" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="AA30" t="inlineStr">
         <is>
-          <t>K1_2</t>
+          <t>K</t>
         </is>
       </c>
       <c r="AB30" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>Mz3</t>
+          <t>Mz</t>
         </is>
       </c>
       <c r="AB46" t="inlineStr">
@@ -11439,7 +11439,7 @@
       </c>
       <c r="AA104" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB104" t="inlineStr"/>
@@ -15045,7 +15045,7 @@
       </c>
       <c r="AA138" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB138" t="inlineStr"/>
@@ -18556,7 +18556,7 @@
       </c>
       <c r="AA171" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB171" t="inlineStr"/>
@@ -18659,7 +18659,7 @@
       </c>
       <c r="AA172" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB172" t="inlineStr"/>
@@ -19083,7 +19083,7 @@
       </c>
       <c r="AA176" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB176" t="inlineStr"/>
@@ -19404,7 +19404,7 @@
       </c>
       <c r="AA179" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB179" t="inlineStr"/>
@@ -22491,7 +22491,7 @@
       </c>
       <c r="AA208" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB208" t="inlineStr"/>
@@ -23216,7 +23216,7 @@
       </c>
       <c r="AA215" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB215" t="inlineStr"/>
@@ -41110,7 +41110,7 @@
       </c>
       <c r="AA385" t="inlineStr">
         <is>
-          <t>J3-K1</t>
+          <t>J-K</t>
         </is>
       </c>
       <c r="AB385" t="inlineStr"/>

</xml_diff>

<commit_message>
adding column with more info about the area
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE477"/>
+  <dimension ref="A1:AF477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,14 +369,14 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Y_UTM</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>X_UTM</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Y_UTM</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>ZoneNumber</t>
@@ -515,6 +515,11 @@
       <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>sampler+year</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>area</t>
         </is>
       </c>
     </row>
@@ -628,6 +633,9 @@
           <t>A.I.Sadovsky,1963</t>
         </is>
       </c>
+      <c r="AF2" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -731,6 +739,9 @@
           <t>A.S.Bochkarev,1984</t>
         </is>
       </c>
+      <c r="AF3" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -834,6 +845,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF4" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -941,6 +955,9 @@
           <t>K.V.laraketsov,1955</t>
         </is>
       </c>
+      <c r="AF5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1044,6 +1061,9 @@
           <t>V.K.Sadakov,1967</t>
         </is>
       </c>
+      <c r="AF6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1147,6 +1167,9 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
+      <c r="AF7" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1250,6 +1273,9 @@
           <t>V.A.Kitaev,1958</t>
         </is>
       </c>
+      <c r="AF8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1357,6 +1383,9 @@
           <t>S.A.Palandzhyan,1976</t>
         </is>
       </c>
+      <c r="AF9" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1464,6 +1493,9 @@
           <t>A.V.Andrianov,1940</t>
         </is>
       </c>
+      <c r="AF10" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1571,6 +1603,9 @@
           <t>I.N.Zubrev,1952</t>
         </is>
       </c>
+      <c r="AF11" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1678,6 +1713,9 @@
           <t>V.N.Lipatov,1958</t>
         </is>
       </c>
+      <c r="AF12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1789,6 +1827,9 @@
           <t>V.I.Noskov,1960</t>
         </is>
       </c>
+      <c r="AF13" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1900,6 +1941,9 @@
           <t>A.O.Andrianov,1939</t>
         </is>
       </c>
+      <c r="AF14" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2003,6 +2047,9 @@
           <t>A.V.Andrianov,1940</t>
         </is>
       </c>
+      <c r="AF15" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2106,6 +2153,9 @@
           <t>E.P.Fedorov,1952</t>
         </is>
       </c>
+      <c r="AF16" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2217,6 +2267,9 @@
           <t>L.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2324,6 +2377,9 @@
           <t>A.P.Shpetny,1947</t>
         </is>
       </c>
+      <c r="AF18" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2431,6 +2487,9 @@
           <t>I.E.Zaedinova,1957</t>
         </is>
       </c>
+      <c r="AF19" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2534,6 +2593,9 @@
           <t>V.I.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF20" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2641,6 +2703,9 @@
           <t>A.K.savel'ev,1950</t>
         </is>
       </c>
+      <c r="AF21" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2744,6 +2809,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF22" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2851,6 +2919,9 @@
           <t>Yu.R.Vasil'ev,1959</t>
         </is>
       </c>
+      <c r="AF23" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2954,6 +3025,9 @@
           <t>G.S.Basiladze,1952</t>
         </is>
       </c>
+      <c r="AF24" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -3065,6 +3139,9 @@
           <t>Z.A.Abdrakhimov,1951</t>
         </is>
       </c>
+      <c r="AF25" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -3172,6 +3249,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF26" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3275,6 +3355,9 @@
           <t>S.A.Palandzhyan,1980</t>
         </is>
       </c>
+      <c r="AF27" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -3374,6 +3457,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF28" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -3477,6 +3563,9 @@
           <t>N.M.Yanchuk,1954</t>
         </is>
       </c>
+      <c r="AF29" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -3580,6 +3669,9 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
+      <c r="AF30" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3687,6 +3779,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF31" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3794,6 +3889,9 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
+      <c r="AF32" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3905,6 +4003,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF33" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -4012,6 +4113,9 @@
           <t>V.I.Teplykh,1964</t>
         </is>
       </c>
+      <c r="AF34" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -4119,6 +4223,9 @@
           <t>A.V.Andrianov,1940</t>
         </is>
       </c>
+      <c r="AF35" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -4226,6 +4333,9 @@
           <t>A.K.Savel'ev,1950</t>
         </is>
       </c>
+      <c r="AF36" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -4333,6 +4443,9 @@
           <t>I.E.Rozhdestvensky,1950</t>
         </is>
       </c>
+      <c r="AF37" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -4440,6 +4553,9 @@
           <t>L.A.Andrianov,1951</t>
         </is>
       </c>
+      <c r="AF38" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -4547,6 +4663,9 @@
           <t>V.A.Zakharov,1961</t>
         </is>
       </c>
+      <c r="AF39" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -4654,6 +4773,9 @@
           <t>A.K.Savel'ev,1949</t>
         </is>
       </c>
+      <c r="AF40" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -4757,6 +4879,9 @@
           <t>E.E.Petrenko,1977</t>
         </is>
       </c>
+      <c r="AF41" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -4864,6 +4989,9 @@
           <t>G.P.Preobrazhensky,1969</t>
         </is>
       </c>
+      <c r="AF42" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -4971,6 +5099,9 @@
           <t>V.A.Ivanov,1967</t>
         </is>
       </c>
+      <c r="AF43" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -5082,6 +5213,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF44" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -5193,6 +5327,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF45" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -5300,6 +5437,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF46" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -5403,6 +5543,9 @@
           <t>V.I.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF47" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -5510,6 +5653,9 @@
           <t>O.N.Ivanov,1971</t>
         </is>
       </c>
+      <c r="AF48" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -5609,6 +5755,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF49" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -5716,6 +5865,9 @@
           <t>I.M.Rusakov,1957</t>
         </is>
       </c>
+      <c r="AF50" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -5827,6 +5979,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF51" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -5930,6 +6085,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF52" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -6041,6 +6199,9 @@
           <t>V.S.Degtyarev,1964</t>
         </is>
       </c>
+      <c r="AF53" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -6152,6 +6313,9 @@
           <t>V.S.Degtyarev,1964</t>
         </is>
       </c>
+      <c r="AF54" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -6255,6 +6419,9 @@
           <t>S.A.Palandzhyan,1976</t>
         </is>
       </c>
+      <c r="AF55" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -6358,6 +6525,9 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
+      <c r="AF56" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -6465,6 +6635,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF57" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -6576,6 +6749,9 @@
           <t>G.S.Basiladze,1952</t>
         </is>
       </c>
+      <c r="AF58" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -6687,6 +6863,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF59" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -6794,6 +6973,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF60" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -6905,6 +7087,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF61" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -7008,6 +7193,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF62" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -7111,6 +7299,9 @@
           <t>I.M.Rusakov,1957</t>
         </is>
       </c>
+      <c r="AF63" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -7222,6 +7413,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF64" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -7325,6 +7519,9 @@
           <t>G.S.Basiladze,1952</t>
         </is>
       </c>
+      <c r="AF65" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -7432,6 +7629,9 @@
           <t>V.l.Shkursky,1962</t>
         </is>
       </c>
+      <c r="AF66" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -7531,6 +7731,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF67" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -7634,6 +7837,9 @@
           <t>V.I.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF68" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -7745,6 +7951,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF69" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -7852,6 +8061,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF70" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -7963,6 +8175,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF71" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -8070,6 +8285,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF72" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -8181,6 +8399,9 @@
           <t>V.I.Noskov,1960</t>
         </is>
       </c>
+      <c r="AF73" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -8284,6 +8505,9 @@
           <t>S.A.Palandzhyan,1976</t>
         </is>
       </c>
+      <c r="AF74" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -8383,6 +8607,9 @@
           <t>I.I.Sonin,1968</t>
         </is>
       </c>
+      <c r="AF75" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -8486,6 +8713,9 @@
           <t>V.I.Kopytin,1961</t>
         </is>
       </c>
+      <c r="AF76" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -8589,6 +8819,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF77" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -8696,6 +8929,9 @@
           <t>O.N.Ivanov,1971</t>
         </is>
       </c>
+      <c r="AF78" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -8803,6 +9039,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF79" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -8914,6 +9153,9 @@
           <t>G.S.Basiladze,1952</t>
         </is>
       </c>
+      <c r="AF80" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -9017,6 +9259,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF81" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -9124,6 +9369,9 @@
           <t>G.B.Zhilinsky,1941</t>
         </is>
       </c>
+      <c r="AF82" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -9231,6 +9479,9 @@
           <t>N.A.Lavrov,1953</t>
         </is>
       </c>
+      <c r="AF83" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -9338,6 +9589,9 @@
           <t>Yu.R.Vasil'ev,1959</t>
         </is>
       </c>
+      <c r="AF84" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -9449,6 +9703,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF85" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -9560,6 +9817,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF86" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -9663,6 +9923,9 @@
           <t>K.L.Bykov,1955</t>
         </is>
       </c>
+      <c r="AF87" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -9766,6 +10029,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF88" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -9865,6 +10131,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF89" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -9964,6 +10233,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF90" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -10071,6 +10343,9 @@
           <t>V.P.Fedorov,1952</t>
         </is>
       </c>
+      <c r="AF91" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -10174,6 +10449,9 @@
           <t>G.M.Sosunov,1958</t>
         </is>
       </c>
+      <c r="AF92" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -10277,6 +10555,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF93" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -10380,6 +10661,9 @@
           <t>O.N.Ivanov,1972</t>
         </is>
       </c>
+      <c r="AF94" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -10487,6 +10771,9 @@
           <t>M.G.Ravich,1938</t>
         </is>
       </c>
+      <c r="AF95" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -10590,6 +10877,9 @@
           <t>V.I.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF96" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -10701,6 +10991,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF97" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -10812,6 +11105,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF98" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -10915,6 +11211,9 @@
           <t>O.N.Ivanov,1979</t>
         </is>
       </c>
+      <c r="AF99" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -11018,6 +11317,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF100" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -11129,6 +11431,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF101" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -11240,6 +11545,9 @@
           <t>G.S.Basiladze,1952</t>
         </is>
       </c>
+      <c r="AF102" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -11351,6 +11659,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF103" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -11454,6 +11765,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF104" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -11561,6 +11875,9 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
+      <c r="AF105" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -11664,6 +11981,9 @@
           <t>O.N.Ivanov,1974</t>
         </is>
       </c>
+      <c r="AF106" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -11771,6 +12091,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF107" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -11878,6 +12201,9 @@
           <t>E.B.Nevretdinov,1972</t>
         </is>
       </c>
+      <c r="AF108" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -11989,6 +12315,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF109" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -12096,6 +12425,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF110" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -12199,6 +12531,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF111" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -12298,6 +12633,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF112" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -12405,6 +12743,9 @@
           <t>M.N.Bogdanov,1967</t>
         </is>
       </c>
+      <c r="AF113" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -12508,6 +12849,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF114" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -12615,6 +12959,9 @@
           <t>V.G.Ditmar,1938</t>
         </is>
       </c>
+      <c r="AF115" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -12726,6 +13073,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF116" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -12837,6 +13187,9 @@
           <t>M.L.Gel'man,1963</t>
         </is>
       </c>
+      <c r="AF117" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -12944,6 +13297,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF118" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -13051,6 +13407,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF119" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -13158,6 +13517,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF120" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -13265,6 +13627,9 @@
           <t>V.G.Silkin,1967</t>
         </is>
       </c>
+      <c r="AF121" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -13368,6 +13733,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF122" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -13479,6 +13847,9 @@
           <t>G.A.Kibanov,1958</t>
         </is>
       </c>
+      <c r="AF123" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -13590,6 +13961,9 @@
           <t>V.A.Kitaev,1958</t>
         </is>
       </c>
+      <c r="AF124" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -13701,6 +14075,9 @@
           <t>V.I.Noskov,1960</t>
         </is>
       </c>
+      <c r="AF125" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -13804,6 +14181,9 @@
           <t>V.P.Pole,1962</t>
         </is>
       </c>
+      <c r="AF126" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -13907,6 +14287,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF127" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -14006,6 +14389,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF128" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -14113,6 +14499,9 @@
           <t>V.G.Ditmar,1938</t>
         </is>
       </c>
+      <c r="AF129" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -14212,6 +14601,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF130" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -14323,6 +14715,9 @@
           <t>V.S.Degtyarev,1962</t>
         </is>
       </c>
+      <c r="AF131" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -14434,6 +14829,9 @@
           <t>O.N.Ivanov,1979</t>
         </is>
       </c>
+      <c r="AF132" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -14537,6 +14935,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF133" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -14644,6 +15045,9 @@
           <t>V.P.Pole,1962</t>
         </is>
       </c>
+      <c r="AF134" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -14747,6 +15151,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF135" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -14846,6 +15253,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF136" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -14957,6 +15367,9 @@
           <t>M.L.Gel'man,1963</t>
         </is>
       </c>
+      <c r="AF137" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -15060,6 +15473,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF138" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -15167,6 +15583,9 @@
           <t>L.A.Andrianov,1951</t>
         </is>
       </c>
+      <c r="AF139" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -15274,6 +15693,9 @@
           <t>A.I.Timoschenko,1960</t>
         </is>
       </c>
+      <c r="AF140" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -15373,6 +15795,9 @@
           <t>I.I.Sonin,1968</t>
         </is>
       </c>
+      <c r="AF141" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -15484,6 +15909,9 @@
           <t>S.A.Palandzhyan,1980</t>
         </is>
       </c>
+      <c r="AF142" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -15591,6 +16019,9 @@
           <t>S.M.Til'man,1956</t>
         </is>
       </c>
+      <c r="AF143" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -15694,6 +16125,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF144" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -15805,6 +16239,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF145" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -15912,6 +16349,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF146" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -16015,6 +16455,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF147" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -16118,6 +16561,9 @@
           <t>A.M.Avdeev,1957</t>
         </is>
       </c>
+      <c r="AF148" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -16221,6 +16667,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF149" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -16324,6 +16773,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF150" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -16427,6 +16879,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF151" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -16538,6 +16993,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF152" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -16649,6 +17107,9 @@
           <t>L.A.Andrianov,1951</t>
         </is>
       </c>
+      <c r="AF153" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -16756,6 +17217,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF154" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -16867,6 +17331,9 @@
           <t>D.S.Golota,1953</t>
         </is>
       </c>
+      <c r="AF155" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -16974,6 +17441,9 @@
           <t>V.I.Teplykh,1964</t>
         </is>
       </c>
+      <c r="AF156" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -17077,6 +17547,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF157" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -17184,6 +17657,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF158" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -17295,6 +17771,9 @@
           <t>A.S.Skalatsky,1964</t>
         </is>
       </c>
+      <c r="AF159" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -17402,6 +17881,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF160" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -17505,6 +17987,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF161" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -17604,6 +18089,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF162" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -17715,6 +18203,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF163" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -17822,6 +18313,9 @@
           <t>L.A.Andrianov,1951</t>
         </is>
       </c>
+      <c r="AF164" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -17933,6 +18427,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF165" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -18040,6 +18537,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF166" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -18151,6 +18651,9 @@
           <t>B.L.Flerov,1958</t>
         </is>
       </c>
+      <c r="AF167" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -18258,6 +18761,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF168" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -18361,6 +18867,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF169" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -18468,6 +18977,9 @@
           <t>V.V.Gulevich,1958</t>
         </is>
       </c>
+      <c r="AF170" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -18571,6 +19083,9 @@
           <t>O.N.Ivanov,1971</t>
         </is>
       </c>
+      <c r="AF171" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -18674,6 +19189,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF172" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -18777,6 +19295,9 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
+      <c r="AF173" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -18884,6 +19405,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF174" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -18995,6 +19519,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF175" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -19098,6 +19625,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF176" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -19205,6 +19735,9 @@
           <t>I.A.Sklyar,1938</t>
         </is>
       </c>
+      <c r="AF177" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -19316,6 +19849,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF178" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -19423,6 +19959,9 @@
           <t>O.N.Ivanov,1971</t>
         </is>
       </c>
+      <c r="AF179" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -19530,6 +20069,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF180" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -19637,6 +20179,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF181" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -19740,6 +20285,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF182" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -19847,6 +20395,9 @@
           <t>A.G.Maltizov,1959</t>
         </is>
       </c>
+      <c r="AF183" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -19954,6 +20505,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF184" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -20057,6 +20611,9 @@
           <t>V.N.Voevodin,1967</t>
         </is>
       </c>
+      <c r="AF185" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -20164,6 +20721,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF186" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -20271,6 +20831,9 @@
           <t>V.A.Kitaev,1958</t>
         </is>
       </c>
+      <c r="AF187" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -20374,6 +20937,9 @@
           <t>V.S.Degtyarev,1966</t>
         </is>
       </c>
+      <c r="AF188" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -20477,6 +21043,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF189" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -20588,6 +21157,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF190" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -20695,6 +21267,9 @@
           <t>D.S.Golota,1953</t>
         </is>
       </c>
+      <c r="AF191" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -20806,6 +21381,9 @@
           <t>A.S.Skalatsky,1960</t>
         </is>
       </c>
+      <c r="AF192" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -20913,6 +21491,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF193" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -21020,6 +21601,9 @@
           <t>P.K.Fedorov,1952</t>
         </is>
       </c>
+      <c r="AF194" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -21123,6 +21707,9 @@
           <t>G.S.Basiladze,1950</t>
         </is>
       </c>
+      <c r="AF195" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -21230,6 +21817,9 @@
           <t>E.B.Nevretdinov,1972</t>
         </is>
       </c>
+      <c r="AF196" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -21341,6 +21931,9 @@
           <t>V.V.Gulevich,1958</t>
         </is>
       </c>
+      <c r="AF197" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -21448,6 +22041,9 @@
           <t>A.M.Demin,1950</t>
         </is>
       </c>
+      <c r="AF198" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -21555,6 +22151,9 @@
           <t>P.K.Fedorov,1952</t>
         </is>
       </c>
+      <c r="AF199" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -21662,6 +22261,9 @@
           <t>A.A.Zhitetsky,1963</t>
         </is>
       </c>
+      <c r="AF200" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -21769,6 +22371,9 @@
           <t>V.V.Gulevich,1958</t>
         </is>
       </c>
+      <c r="AF201" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -21868,6 +22473,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF202" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -21971,6 +22579,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF203" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -22082,6 +22693,9 @@
           <t>G.I.Bogomolov,1965</t>
         </is>
       </c>
+      <c r="AF204" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -22189,6 +22803,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF205" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -22296,6 +22913,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF206" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -22403,6 +23023,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF207" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -22506,6 +23129,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF208" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -22609,6 +23235,9 @@
           <t>V.G.Zheltovsky,1972</t>
         </is>
       </c>
+      <c r="AF209" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -22716,6 +23345,9 @@
           <t>S.P.Skuratovsky,1966</t>
         </is>
       </c>
+      <c r="AF210" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -22815,6 +23447,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF211" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -22918,6 +23553,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF212" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -23021,6 +23659,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF213" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -23128,6 +23769,9 @@
           <t>D.S.Golota,1953</t>
         </is>
       </c>
+      <c r="AF214" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -23231,6 +23875,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF215" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -23338,6 +23985,9 @@
           <t>Yu.P.Misans,1956</t>
         </is>
       </c>
+      <c r="AF216" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -23441,6 +24091,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF217" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -23548,6 +24201,9 @@
           <t>V.I.Teplykh,1963</t>
         </is>
       </c>
+      <c r="AF218" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -23655,6 +24311,9 @@
           <t>V.l.Shkursky,1966</t>
         </is>
       </c>
+      <c r="AF219" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -23758,6 +24417,9 @@
           <t>N.N.Tevyashov,1966</t>
         </is>
       </c>
+      <c r="AF220" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -23865,6 +24527,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF221" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -23972,6 +24637,9 @@
           <t>A.I.Grigor'ev,1961</t>
         </is>
       </c>
+      <c r="AF222" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -24079,6 +24747,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF223" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -24186,6 +24857,9 @@
           <t>V.G.Ditmar,1938</t>
         </is>
       </c>
+      <c r="AF224" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -24297,6 +24971,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF225" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -24408,6 +25085,9 @@
           <t>V.G.Zheltovsky,1974</t>
         </is>
       </c>
+      <c r="AF226" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -24519,6 +25199,9 @@
           <t>V.S.Smolich,1947</t>
         </is>
       </c>
+      <c r="AF227" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -24626,6 +25309,9 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
+      <c r="AF228" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -24729,6 +25415,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF229" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -24836,6 +25525,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF230" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -24935,6 +25627,9 @@
           <t>N.I.Filatova,1967</t>
         </is>
       </c>
+      <c r="AF231" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -25042,6 +25737,9 @@
           <t>N.I.Tikhomirov,1940</t>
         </is>
       </c>
+      <c r="AF232" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -25145,6 +25843,9 @@
           <t>N.N.Tevyashov,1966</t>
         </is>
       </c>
+      <c r="AF233" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -25248,6 +25949,9 @@
           <t>I.N.Trumpe,1958</t>
         </is>
       </c>
+      <c r="AF234" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -25351,6 +26055,9 @@
           <t>O.N.Ivanov,1972</t>
         </is>
       </c>
+      <c r="AF235" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -25454,6 +26161,9 @@
           <t>S.P.Skuratovsky,1966</t>
         </is>
       </c>
+      <c r="AF236" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -25561,6 +26271,9 @@
           <t>V.I.Shkursky,1966</t>
         </is>
       </c>
+      <c r="AF237" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -25660,6 +26373,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF238" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -25763,6 +26479,9 @@
           <t>G.M.Sosunov,1958</t>
         </is>
       </c>
+      <c r="AF239" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -25870,6 +26589,9 @@
           <t>G.B.Zhilinsky,1941</t>
         </is>
       </c>
+      <c r="AF240" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -25977,6 +26699,9 @@
           <t>N.I.Tikhomirov,1938</t>
         </is>
       </c>
+      <c r="AF241" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -26076,6 +26801,9 @@
           <t>E.K.Zotov,1965</t>
         </is>
       </c>
+      <c r="AF242" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -26183,6 +26911,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF243" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -26286,6 +27017,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF244" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -26393,6 +27127,9 @@
           <t>G.A.Kremchukov,1936</t>
         </is>
       </c>
+      <c r="AF245" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -26496,6 +27233,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF246" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -26599,6 +27339,9 @@
           <t>N.N.Neznanov,1964</t>
         </is>
       </c>
+      <c r="AF247" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -26702,6 +27445,9 @@
           <t>Yu.K.Usenko,1963</t>
         </is>
       </c>
+      <c r="AF248" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -26805,6 +27551,9 @@
           <t>G.M.Dautov,1940</t>
         </is>
       </c>
+      <c r="AF249" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -26916,6 +27665,9 @@
           <t>V.S.Bogoyavlensky,1964</t>
         </is>
       </c>
+      <c r="AF250" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -27019,6 +27771,9 @@
           <t>A.S.Ulitin</t>
         </is>
       </c>
+      <c r="AF251" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -27126,6 +27881,9 @@
           <t>V.V.Gulevich,1963</t>
         </is>
       </c>
+      <c r="AF252" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -27237,6 +27995,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF253" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -27344,6 +28105,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF254" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -27451,6 +28215,9 @@
           <t>N.Vorob'ev's coll.,1977</t>
         </is>
       </c>
+      <c r="AF255" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -27558,6 +28325,9 @@
           <t>B.L.Flerov,1958</t>
         </is>
       </c>
+      <c r="AF256" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -27665,6 +28435,9 @@
           <t>V.V.Isaev,1963</t>
         </is>
       </c>
+      <c r="AF257" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -27772,6 +28545,9 @@
           <t>G.B.Zhilinsky,1941</t>
         </is>
       </c>
+      <c r="AF258" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -27875,6 +28651,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF259" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -27978,6 +28757,9 @@
           <t>M.O.Chasovitov,1959</t>
         </is>
       </c>
+      <c r="AF260" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -28081,6 +28863,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF261" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -28184,6 +28969,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF262" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -28287,6 +29075,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF263" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -28394,6 +29185,9 @@
           <t>V.P.Pole,1962</t>
         </is>
       </c>
+      <c r="AF264" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -28505,6 +29299,9 @@
           <t>A.S.Skalatsky,1964</t>
         </is>
       </c>
+      <c r="AF265" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -28612,6 +29409,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF266" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -28715,6 +29515,9 @@
           <t>V.I.Kopytin,1961</t>
         </is>
       </c>
+      <c r="AF267" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -28826,6 +29629,9 @@
           <t>V.S.Smolich,1947</t>
         </is>
       </c>
+      <c r="AF268" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -28929,6 +29735,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF269" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -29032,6 +29841,9 @@
           <t>G.A.Klimov,1960</t>
         </is>
       </c>
+      <c r="AF270" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -29143,6 +29955,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF271" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -29250,6 +30065,9 @@
           <t>A.I.Grigor'ev,1965</t>
         </is>
       </c>
+      <c r="AF272" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -29349,6 +30167,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF273" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -29452,6 +30273,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF274" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -29555,6 +30379,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF275" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -29662,6 +30489,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF276" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -29765,6 +30595,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF277" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -29872,6 +30705,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF278" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -29983,6 +30819,9 @@
           <t>V.I.Noskov,1957</t>
         </is>
       </c>
+      <c r="AF279" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -30082,6 +30921,9 @@
           <t>V.I.Shavel',1967</t>
         </is>
       </c>
+      <c r="AF280" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -30189,6 +31031,9 @@
           <t>Ya.P.Misans,1956</t>
         </is>
       </c>
+      <c r="AF281" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -30292,6 +31137,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF282" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -30399,6 +31247,9 @@
           <t>A.G.Maltizov,1959</t>
         </is>
       </c>
+      <c r="AF283" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -30506,6 +31357,9 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
+      <c r="AF284" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -30613,6 +31467,9 @@
           <t>A.S.Monyakin,1954</t>
         </is>
       </c>
+      <c r="AF285" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -30716,6 +31573,9 @@
           <t>P.P.Ushakov,1940</t>
         </is>
       </c>
+      <c r="AF286" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -30827,6 +31687,9 @@
           <t>V.S.Bogoyavlensky,1964</t>
         </is>
       </c>
+      <c r="AF287" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -30930,6 +31793,9 @@
           <t>V.I.Shavel',1967</t>
         </is>
       </c>
+      <c r="AF288" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -31037,6 +31903,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF289" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -31144,6 +32013,9 @@
           <t>R.M.Beschastnaya,1962</t>
         </is>
       </c>
+      <c r="AF290" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -31243,6 +32115,9 @@
           <t>N.I.Filatova,1967</t>
         </is>
       </c>
+      <c r="AF291" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -31346,6 +32221,9 @@
           <t>G.B.Zhilinsky,1941</t>
         </is>
       </c>
+      <c r="AF292" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -31453,6 +32331,9 @@
           <t>R.M.Beschastnova,1962</t>
         </is>
       </c>
+      <c r="AF293" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -31564,6 +32445,9 @@
           <t>N.N.Neznanov,1959</t>
         </is>
       </c>
+      <c r="AF294" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -31667,6 +32551,9 @@
           <t>A.Ya.Radzivill,1965</t>
         </is>
       </c>
+      <c r="AF295" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -31774,6 +32661,9 @@
           <t>A.K.Savel'ev,1949</t>
         </is>
       </c>
+      <c r="AF296" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -31885,6 +32775,9 @@
           <t>V.S.Bogoyavlensky,1964</t>
         </is>
       </c>
+      <c r="AF297" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -31992,6 +32885,9 @@
           <t>V.A.Shkursky,1962</t>
         </is>
       </c>
+      <c r="AF298" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -32099,6 +32995,9 @@
           <t>L.I.Sereda,1966</t>
         </is>
       </c>
+      <c r="AF299" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -32206,6 +33105,9 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
+      <c r="AF300" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -32309,6 +33211,9 @@
           <t>G.B.Zhilinsky,1940</t>
         </is>
       </c>
+      <c r="AF301" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -32420,6 +33325,9 @@
           <t>A.M.Demin,1950</t>
         </is>
       </c>
+      <c r="AF302" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -32531,6 +33439,9 @@
           <t>B.L.Flerov,1958</t>
         </is>
       </c>
+      <c r="AF303" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -32642,6 +33553,9 @@
           <t>V.I.Teplykh,1963</t>
         </is>
       </c>
+      <c r="AF304" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -32749,6 +33663,9 @@
           <t>V.S.Degtyarev,1960</t>
         </is>
       </c>
+      <c r="AF305" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -32852,6 +33769,9 @@
           <t>V.G.Zheltovsky,1975</t>
         </is>
       </c>
+      <c r="AF306" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -32959,6 +33879,9 @@
           <t>A.Ya.Radzivill,1960</t>
         </is>
       </c>
+      <c r="AF307" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -33066,6 +33989,9 @@
           <t>D.F.Egorov,1957</t>
         </is>
       </c>
+      <c r="AF308" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -33177,6 +34103,9 @@
           <t>A.I.Grigor'ev,1965</t>
         </is>
       </c>
+      <c r="AF309" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -33280,6 +34209,9 @@
           <t>M.I.Rokhlin,1930</t>
         </is>
       </c>
+      <c r="AF310" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -33379,6 +34311,9 @@
           <t>V.I.Shavel',1967</t>
         </is>
       </c>
+      <c r="AF311" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -33482,6 +34417,9 @@
           <t>V.G.Zheltovsky,1973</t>
         </is>
       </c>
+      <c r="AF312" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -33589,6 +34527,9 @@
           <t>B.D.Trunov,1963</t>
         </is>
       </c>
+      <c r="AF313" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -33696,6 +34637,9 @@
           <t>A.G.Senotrusov,1964</t>
         </is>
       </c>
+      <c r="AF314" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -33803,6 +34747,9 @@
           <t>A.S.Bochkarev,l984</t>
         </is>
       </c>
+      <c r="AF315" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -33906,6 +34853,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF316" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -34009,6 +34959,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF317" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -34120,6 +35073,9 @@
           <t>S.G.Zhelnina'1957</t>
         </is>
       </c>
+      <c r="AF318" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -34223,6 +35179,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF319" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -34326,6 +35285,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF320" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -34437,6 +35399,9 @@
           <t>D.S.Golota,1953</t>
         </is>
       </c>
+      <c r="AF321" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -34548,6 +35513,9 @@
           <t>V.A.Zakharov,1958</t>
         </is>
       </c>
+      <c r="AF322" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -34651,6 +35619,9 @@
           <t>Yu.M.Dovgal',1962</t>
         </is>
       </c>
+      <c r="AF323" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -34758,6 +35729,9 @@
           <t>M.I.Rokhlin,1936</t>
         </is>
       </c>
+      <c r="AF324" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -34869,6 +35843,9 @@
           <t>B.L.Flerov,1959</t>
         </is>
       </c>
+      <c r="AF325" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -34972,6 +35949,9 @@
           <t>V.A.Kitaev,1963</t>
         </is>
       </c>
+      <c r="AF326" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -35075,6 +36055,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF327" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -35182,6 +36165,9 @@
           <t>V.P.Vasilenko,1966</t>
         </is>
       </c>
+      <c r="AF328" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -35285,6 +36271,9 @@
           <t>S.G.Zhelnina,1965</t>
         </is>
       </c>
+      <c r="AF329" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -35388,6 +36377,9 @@
           <t>M.I.Rokhlin,1937</t>
         </is>
       </c>
+      <c r="AF330" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -35491,6 +36483,9 @@
           <t>A.K.Savel'ev,1949</t>
         </is>
       </c>
+      <c r="AF331" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -35590,6 +36585,9 @@
           <t>A.A.Alekseev,1968</t>
         </is>
       </c>
+      <c r="AF332" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -35697,6 +36695,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF333" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -35796,6 +36797,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF334" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -35907,6 +36911,9 @@
           <t>A.V.Andrianov,1940</t>
         </is>
       </c>
+      <c r="AF335" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -36010,6 +37017,9 @@
           <t>G.V.Zhilinsky,1940</t>
         </is>
       </c>
+      <c r="AF336" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -36113,6 +37123,9 @@
           <t>N.M.Keppen,1941</t>
         </is>
       </c>
+      <c r="AF337" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -36212,6 +37225,9 @@
           <t>E.G.Bordyugov,1978</t>
         </is>
       </c>
+      <c r="AF338" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -36323,6 +37339,9 @@
           <t>B.L.Flerov,1958</t>
         </is>
       </c>
+      <c r="AF339" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -36434,6 +37453,9 @@
           <t>A.M.Demin,1950</t>
         </is>
       </c>
+      <c r="AF340" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -36537,6 +37559,9 @@
           <t>A.G.Senotrusov,1965</t>
         </is>
       </c>
+      <c r="AF341" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -36644,6 +37669,9 @@
           <t>V.I.Shkursky,1962</t>
         </is>
       </c>
+      <c r="AF342" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -36743,6 +37771,9 @@
           <t>A.A.Alekseev 1968</t>
         </is>
       </c>
+      <c r="AF343" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -36850,6 +37881,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF344" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -36953,6 +37987,9 @@
           <t>B.F.Palymsky,1964</t>
         </is>
       </c>
+      <c r="AF345" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -37052,6 +38089,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF346" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -37159,6 +38199,9 @@
           <t>A.G.Maltizov,1959</t>
         </is>
       </c>
+      <c r="AF347" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -37266,6 +38309,9 @@
           <t>I.I.Akramovsky,1960</t>
         </is>
       </c>
+      <c r="AF348" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -37373,6 +38419,9 @@
           <t>V.S.Degtyarev,1961</t>
         </is>
       </c>
+      <c r="AF349" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -37484,6 +38533,9 @@
           <t>A.M.Demin,1950</t>
         </is>
       </c>
+      <c r="AF350" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -37587,6 +38639,9 @@
           <t>S.P.Skuratovsky,1966</t>
         </is>
       </c>
+      <c r="AF351" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -37694,6 +38749,9 @@
           <t>M.N.Kozhemyako,1947</t>
         </is>
       </c>
+      <c r="AF352" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -37797,6 +38855,9 @@
           <t>M.I.Rokhlin,1937</t>
         </is>
       </c>
+      <c r="AF353" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -37900,6 +38961,9 @@
           <t>V.V.Gulevich,1963</t>
         </is>
       </c>
+      <c r="AF354" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -38011,6 +39075,9 @@
           <t>V.S.Degtyarev,1964</t>
         </is>
       </c>
+      <c r="AF355" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -38114,6 +39181,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF356" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -38213,6 +39283,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF357" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -38324,6 +39397,9 @@
           <t>I.A.Yudakov,1959</t>
         </is>
       </c>
+      <c r="AF358" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -38431,6 +39507,9 @@
           <t>B.M.Flerov,1953</t>
         </is>
       </c>
+      <c r="AF359" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -38534,6 +39613,9 @@
           <t>O.N.Ivanov,1972</t>
         </is>
       </c>
+      <c r="AF360" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -38645,6 +39727,9 @@
           <t>G.A.Kibanov,1958</t>
         </is>
       </c>
+      <c r="AF361" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -38748,6 +39833,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF362" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -38855,6 +39943,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF363" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -38962,6 +40053,9 @@
           <t>N.N.Zlobin,1941</t>
         </is>
       </c>
+      <c r="AF364" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -39061,6 +40155,9 @@
           <t>E.K.Zotov,1965</t>
         </is>
       </c>
+      <c r="AF365" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -39164,6 +40261,9 @@
           <t>M.I.Rokhlin,1938</t>
         </is>
       </c>
+      <c r="AF366" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -39275,6 +40375,9 @@
           <t>B.L.Flerov,1959</t>
         </is>
       </c>
+      <c r="AF367" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -39378,6 +40481,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF368" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -39485,6 +40591,9 @@
           <t>G.P.Preobrazhensky,1969</t>
         </is>
       </c>
+      <c r="AF369" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -39588,6 +40697,9 @@
           <t>N.M.Zlobin,1941</t>
         </is>
       </c>
+      <c r="AF370" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -39691,6 +40803,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF371" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -39790,6 +40905,9 @@
           <t>E.K.Zotov,1965</t>
         </is>
       </c>
+      <c r="AF372" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -39889,6 +41007,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF373" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -39996,6 +41117,9 @@
           <t>G.I.Bogomolov'1965</t>
         </is>
       </c>
+      <c r="AF374" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -40099,6 +41223,9 @@
           <t>O.N.Ivanov,1972</t>
         </is>
       </c>
+      <c r="AF375" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
@@ -40206,6 +41333,9 @@
           <t>V.A.Ivanov,1967</t>
         </is>
       </c>
+      <c r="AF376" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -40305,6 +41435,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF377" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
@@ -40408,6 +41541,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF378" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
@@ -40511,6 +41647,9 @@
           <t>G.B.Zhilinsky,1940</t>
         </is>
       </c>
+      <c r="AF379" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -40614,6 +41753,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF380" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
@@ -40713,6 +41855,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF381" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
@@ -40812,6 +41957,9 @@
           <t>Yu.I.Evstaf'ev,1966</t>
         </is>
       </c>
+      <c r="AF382" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
@@ -40915,6 +42063,9 @@
           <t>V.A.Ivanov,1967</t>
         </is>
       </c>
+      <c r="AF383" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -41022,6 +42173,9 @@
           <t>A.I.Timoschenko,1960</t>
         </is>
       </c>
+      <c r="AF384" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
@@ -41125,6 +42279,9 @@
           <t>O.N.Ivanov,1977</t>
         </is>
       </c>
+      <c r="AF385" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
@@ -41228,6 +42385,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF386" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
@@ -41335,6 +42495,9 @@
           <t>M.I.Rabkin,1940</t>
         </is>
       </c>
+      <c r="AF387" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
@@ -41442,6 +42605,9 @@
           <t>M.N.Zlobin,1941</t>
         </is>
       </c>
+      <c r="AF388" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
@@ -41541,6 +42707,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF389" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
@@ -41648,6 +42817,9 @@
           <t>G.P.Preobrazhensky,1969</t>
         </is>
       </c>
+      <c r="AF390" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -41747,6 +42919,9 @@
           <t>N.I.Filatova,1967</t>
         </is>
       </c>
+      <c r="AF391" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
@@ -41854,6 +43029,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF392" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
@@ -41957,6 +43135,9 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
+      <c r="AF393" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
@@ -42068,6 +43249,9 @@
           <t>A.M.Demin,1950</t>
         </is>
       </c>
+      <c r="AF394" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
@@ -42171,6 +43355,9 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
+      <c r="AF395" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
@@ -42282,6 +43469,9 @@
           <t>A.S.Skalatsky,1960</t>
         </is>
       </c>
+      <c r="AF396" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
@@ -42385,6 +43575,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF397" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
@@ -42496,6 +43689,9 @@
           <t>V.S.Degtyarev,1964</t>
         </is>
       </c>
+      <c r="AF398" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
@@ -42603,6 +43799,9 @@
           <t>A.G.Senotrusov,1965</t>
         </is>
       </c>
+      <c r="AF399" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
@@ -42702,6 +43901,9 @@
           <t>S.S.Lobunetz,1972</t>
         </is>
       </c>
+      <c r="AF400" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -42805,6 +44007,9 @@
           <t>S.P.Skuratovsky,1966</t>
         </is>
       </c>
+      <c r="AF401" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" s="1" t="n">
@@ -42916,6 +44121,9 @@
           <t>A.I.Sadovsky,1963</t>
         </is>
       </c>
+      <c r="AF402" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" s="1" t="n">
@@ -43019,6 +44227,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF403" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" s="1" t="n">
@@ -43126,6 +44337,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF404" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" s="1" t="n">
@@ -43225,6 +44439,9 @@
           <t>E.K.Zotov,1964</t>
         </is>
       </c>
+      <c r="AF405" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -43324,6 +44541,9 @@
           <t>I.I.Sonin,1968</t>
         </is>
       </c>
+      <c r="AF406" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
@@ -43427,6 +44647,9 @@
           <t>M.I.Rokhlin,1938</t>
         </is>
       </c>
+      <c r="AF407" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="n">
@@ -43534,6 +44757,9 @@
           <t>R.M.Dautov,1940</t>
         </is>
       </c>
+      <c r="AF408" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
@@ -43637,6 +44863,9 @@
           <t>N.M.Keppen,1940</t>
         </is>
       </c>
+      <c r="AF409" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
@@ -43744,6 +44973,9 @@
           <t>V.A.Ivanov,1967</t>
         </is>
       </c>
+      <c r="AF410" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" s="1" t="n">
@@ -43847,6 +45079,9 @@
           <t>S.M.Til'man,1956</t>
         </is>
       </c>
+      <c r="AF411" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -43950,6 +45185,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF412" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" s="1" t="n">
@@ -44057,6 +45295,9 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
+      <c r="AF413" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" s="1" t="n">
@@ -44160,6 +45401,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF414" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" s="1" t="n">
@@ -44259,6 +45503,9 @@
           <t>V.I.Shavel',1967</t>
         </is>
       </c>
+      <c r="AF415" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="n">
@@ -44366,6 +45613,9 @@
           <t>A.P.Shpetny,1948</t>
         </is>
       </c>
+      <c r="AF416" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="n">
@@ -44469,6 +45719,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF417" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -44572,6 +45825,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF418" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" s="1" t="n">
@@ -44679,6 +45935,9 @@
           <t>L.M.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF419" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
@@ -44778,6 +46037,9 @@
           <t>G.I.Agal'tsov,1961</t>
         </is>
       </c>
+      <c r="AF420" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
@@ -44881,6 +46143,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF421" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" s="1" t="n">
@@ -44988,6 +46253,9 @@
           <t>V.I.Shkursky,1962</t>
         </is>
       </c>
+      <c r="AF422" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
@@ -45099,6 +46367,9 @@
           <t>Vlodavetz,1932</t>
         </is>
       </c>
+      <c r="AF423" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="424">
       <c r="A424" s="1" t="n">
@@ -45206,6 +46477,9 @@
           <t>M.N.Bogdanova,1967</t>
         </is>
       </c>
+      <c r="AF424" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" s="1" t="n">
@@ -45313,6 +46587,9 @@
           <t>I.I.Akramovsky,1960</t>
         </is>
       </c>
+      <c r="AF425" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
@@ -45412,6 +46689,9 @@
           <t>A.A.Alekseev,1968</t>
         </is>
       </c>
+      <c r="AF426" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -45511,6 +46791,9 @@
           <t>A.S.Bochkarev,1984</t>
         </is>
       </c>
+      <c r="AF427" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
@@ -45610,6 +46893,9 @@
           <t>V.I.Shavel',1967</t>
         </is>
       </c>
+      <c r="AF428" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="429">
       <c r="A429" s="1" t="n">
@@ -45717,6 +47003,9 @@
           <t>G.P.Preobrazhensky,1969</t>
         </is>
       </c>
+      <c r="AF429" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" s="1" t="n">
@@ -45820,6 +47109,9 @@
           <t>R.M.Dautov,1940</t>
         </is>
       </c>
+      <c r="AF430" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="431">
       <c r="A431" s="1" t="n">
@@ -45927,6 +47219,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF431" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="432">
       <c r="A432" s="1" t="n">
@@ -46034,6 +47329,9 @@
           <t>K.S.Sukhov,1964</t>
         </is>
       </c>
+      <c r="AF432" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="433">
       <c r="A433" s="1" t="n">
@@ -46145,6 +47443,9 @@
           <t>M.I.Gel'man,1960</t>
         </is>
       </c>
+      <c r="AF433" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="434">
       <c r="A434" s="1" t="n">
@@ -46248,6 +47549,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF434" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="435">
       <c r="A435" s="1" t="n">
@@ -46355,6 +47659,9 @@
           <t>N.M.Zlobin,1941</t>
         </is>
       </c>
+      <c r="AF435" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="436">
       <c r="A436" s="1" t="n">
@@ -46458,6 +47765,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF436" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
@@ -46561,6 +47871,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF437" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="438">
       <c r="A438" s="1" t="n">
@@ -46664,6 +47977,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF438" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
@@ -46767,6 +48083,9 @@
           <t>A.S.Bochkarev,1984</t>
         </is>
       </c>
+      <c r="AF439" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="440">
       <c r="A440" s="1" t="n">
@@ -46870,6 +48189,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF440" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="441">
       <c r="A441" s="1" t="n">
@@ -46977,6 +48299,9 @@
           <t>I.E.Zaedinova,1957</t>
         </is>
       </c>
+      <c r="AF441" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="442">
       <c r="A442" s="1" t="n">
@@ -47088,6 +48413,9 @@
           <t>G.K.Kleschev,1958</t>
         </is>
       </c>
+      <c r="AF442" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="443">
       <c r="A443" s="1" t="n">
@@ -47191,6 +48519,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF443" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="444">
       <c r="A444" s="1" t="n">
@@ -47294,6 +48625,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF444" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="445">
       <c r="A445" s="1" t="n">
@@ -47397,6 +48731,9 @@
           <t>E.G.Bordyugov,1973</t>
         </is>
       </c>
+      <c r="AF445" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="446">
       <c r="A446" s="1" t="n">
@@ -47500,6 +48837,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF446" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="447">
       <c r="A447" s="1" t="n">
@@ -47607,6 +48947,9 @@
           <t>S.P.Skuratovsky,1966</t>
         </is>
       </c>
+      <c r="AF447" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
@@ -47714,6 +49057,9 @@
           <t>V.P.Vasilenko,1966</t>
         </is>
       </c>
+      <c r="AF448" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="449">
       <c r="A449" s="1" t="n">
@@ -47817,6 +49163,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF449" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
@@ -47920,6 +49269,9 @@
           <t>S.G.Belobzhinsky's coll.,1973</t>
         </is>
       </c>
+      <c r="AF450" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="451">
       <c r="A451" s="1" t="n">
@@ -48023,6 +49375,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF451" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="452">
       <c r="A452" s="1" t="n">
@@ -48130,6 +49485,9 @@
           <t>V.l.Shkursky,1962</t>
         </is>
       </c>
+      <c r="AF452" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="453">
       <c r="A453" s="1" t="n">
@@ -48229,6 +49587,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF453" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="454">
       <c r="A454" s="1" t="n">
@@ -48328,6 +49689,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF454" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="455">
       <c r="A455" s="1" t="n">
@@ -48431,6 +49795,9 @@
           <t>A.B.Tsukernik,1969</t>
         </is>
       </c>
+      <c r="AF455" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="456">
       <c r="A456" s="1" t="n">
@@ -48530,6 +49897,9 @@
           <t>I.M.Mertsalov,1969</t>
         </is>
       </c>
+      <c r="AF456" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="457">
       <c r="A457" s="1" t="n">
@@ -48637,6 +50007,9 @@
           <t>A.V.Volokhin,1963</t>
         </is>
       </c>
+      <c r="AF457" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="458">
       <c r="A458" s="1" t="n">
@@ -48740,6 +50113,9 @@
           <t>V.A.Kasatkin,1963</t>
         </is>
       </c>
+      <c r="AF458" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="459">
       <c r="A459" s="1" t="n">
@@ -48847,6 +50223,9 @@
           <t>Yu.A.Novoselov,1968</t>
         </is>
       </c>
+      <c r="AF459" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="460">
       <c r="A460" s="1" t="n">
@@ -48950,6 +50329,9 @@
           <t>A.S.Bochkarev,1984</t>
         </is>
       </c>
+      <c r="AF460" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="461">
       <c r="A461" s="1" t="n">
@@ -49049,6 +50431,9 @@
           <t>Yu.I.Evstaf'ev,1966</t>
         </is>
       </c>
+      <c r="AF461" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="462">
       <c r="A462" s="1" t="n">
@@ -49148,6 +50533,9 @@
           <t>N.I.Filatova,1968</t>
         </is>
       </c>
+      <c r="AF462" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="463">
       <c r="A463" s="1" t="n">
@@ -49247,6 +50635,9 @@
           <t>A.A.Alekseev,1968</t>
         </is>
       </c>
+      <c r="AF463" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="464">
       <c r="A464" s="1" t="n">
@@ -49350,6 +50741,9 @@
           <t>L.I.Karpasov,1965</t>
         </is>
       </c>
+      <c r="AF464" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="465">
       <c r="A465" s="1" t="n">
@@ -49449,6 +50843,9 @@
           <t>I.M.Mertsalov,1969</t>
         </is>
       </c>
+      <c r="AF465" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="466">
       <c r="A466" s="1" t="n">
@@ -49552,6 +50949,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF466" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="467">
       <c r="A467" s="1" t="n">
@@ -49659,6 +51059,9 @@
           <t>A.G.Senotrusov,1965</t>
         </is>
       </c>
+      <c r="AF467" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="468">
       <c r="A468" s="1" t="n">
@@ -49762,6 +51165,9 @@
           <t>N.I.Filatova,1967</t>
         </is>
       </c>
+      <c r="AF468" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="469">
       <c r="A469" s="1" t="n">
@@ -49873,6 +51279,9 @@
           <t>L.l.Sereda,1966</t>
         </is>
       </c>
+      <c r="AF469" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="470">
       <c r="A470" s="1" t="n">
@@ -49980,6 +51389,9 @@
           <t>Yu.A.Novoselov,1968</t>
         </is>
       </c>
+      <c r="AF470" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="471">
       <c r="A471" s="1" t="n">
@@ -50083,6 +51495,9 @@
           <t>V.A.Faradzhev,1971</t>
         </is>
       </c>
+      <c r="AF471" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="472">
       <c r="A472" s="1" t="n">
@@ -50186,6 +51601,9 @@
           <t>A.G.Senotrusov,1965</t>
         </is>
       </c>
+      <c r="AF472" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="473">
       <c r="A473" s="1" t="n">
@@ -50285,6 +51703,9 @@
           <t>A.A.Alekseev,1968</t>
         </is>
       </c>
+      <c r="AF473" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="474">
       <c r="A474" s="1" t="n">
@@ -50388,6 +51809,9 @@
           <t>S.S.Lobunetz,1968</t>
         </is>
       </c>
+      <c r="AF474" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="475">
       <c r="A475" s="1" t="n">
@@ -50487,6 +51911,9 @@
           <t>E.A.Struve,1940</t>
         </is>
       </c>
+      <c r="AF475" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="476">
       <c r="A476" s="1" t="n">
@@ -50594,6 +52021,9 @@
           <t>V.A.lgnat'ev,1964</t>
         </is>
       </c>
+      <c r="AF476" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="477">
       <c r="A477" s="1" t="n">
@@ -50704,6 +52134,9 @@
         <is>
           <t>M.G.Ravich,1938</t>
         </is>
+      </c>
+      <c r="AF477" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4/04 optimizing variogram parameters for area3
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -864,7 +864,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3582,7 +3582,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4242,7 +4242,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4352,7 +4352,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5232,7 +5232,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5884,7 +5884,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6104,7 +6104,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6218,7 +6218,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6544,7 +6544,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6768,7 +6768,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6882,7 +6882,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6992,7 +6992,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7106,7 +7106,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7212,7 +7212,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7318,7 +7318,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7432,7 +7432,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7648,7 +7648,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7750,7 +7750,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7856,7 +7856,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7970,7 +7970,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8080,7 +8080,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8194,7 +8194,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8304,7 +8304,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8418,7 +8418,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8524,7 +8524,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8626,7 +8626,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8732,7 +8732,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8838,7 +8838,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8948,7 +8948,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9058,7 +9058,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9172,7 +9172,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9278,7 +9278,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9388,7 +9388,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9498,7 +9498,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9608,7 +9608,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9722,7 +9722,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9836,7 +9836,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9942,7 +9942,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10048,7 +10048,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10252,7 +10252,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10362,7 +10362,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10468,7 +10468,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10574,7 +10574,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10680,7 +10680,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10790,7 +10790,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10896,7 +10896,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11010,7 +11010,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11124,7 +11124,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11230,7 +11230,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11344,7 +11344,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11458,7 +11458,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11572,7 +11572,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11678,7 +11678,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11788,7 +11788,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11894,7 +11894,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12004,7 +12004,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12114,7 +12114,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12228,7 +12228,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12338,7 +12338,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12444,7 +12444,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12546,7 +12546,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -12656,7 +12656,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12762,7 +12762,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12872,7 +12872,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12986,7 +12986,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13100,7 +13100,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13210,7 +13210,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13320,7 +13320,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13536,7 +13536,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -13650,7 +13650,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13764,7 +13764,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13878,7 +13878,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13984,7 +13984,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14090,7 +14090,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14192,7 +14192,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14302,7 +14302,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14404,7 +14404,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14518,7 +14518,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -14632,7 +14632,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -14738,7 +14738,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14848,7 +14848,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14954,7 +14954,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15056,7 +15056,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15170,7 +15170,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15276,7 +15276,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15386,7 +15386,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -15496,7 +15496,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -15598,7 +15598,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -15712,7 +15712,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -15822,7 +15822,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15928,7 +15928,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16042,7 +16042,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16152,7 +16152,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16258,7 +16258,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16364,7 +16364,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -16470,7 +16470,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -16576,7 +16576,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -16682,7 +16682,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -16796,7 +16796,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16910,7 +16910,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17024,7 +17024,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17134,7 +17134,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17240,7 +17240,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17350,7 +17350,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -17464,7 +17464,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -17574,7 +17574,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -17680,7 +17680,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -17782,7 +17782,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -17896,7 +17896,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18006,7 +18006,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18120,7 +18120,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18234,7 +18234,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18344,7 +18344,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -18450,7 +18450,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -18560,7 +18560,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -18666,7 +18666,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -18772,7 +18772,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -18878,7 +18878,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -18988,7 +18988,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19102,7 +19102,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19208,7 +19208,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19318,7 +19318,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -19432,7 +19432,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -19542,7 +19542,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -19652,7 +19652,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -19762,7 +19762,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -19868,7 +19868,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -19978,7 +19978,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -20088,7 +20088,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -20194,7 +20194,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -20304,7 +20304,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -20410,7 +20410,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -20516,7 +20516,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -20630,7 +20630,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -20740,7 +20740,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -20854,7 +20854,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -20964,7 +20964,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -21074,7 +21074,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -21180,7 +21180,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -21290,7 +21290,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -21404,7 +21404,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -21514,7 +21514,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -21624,7 +21624,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -21734,7 +21734,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -21844,7 +21844,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -21946,7 +21946,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -22052,7 +22052,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -22166,7 +22166,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -22276,7 +22276,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -22386,7 +22386,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -22492,7 +22492,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -22598,7 +22598,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -22708,7 +22708,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -22810,7 +22810,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -22916,7 +22916,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -23022,7 +23022,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -23132,7 +23132,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -23238,7 +23238,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -23348,7 +23348,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -23454,7 +23454,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -23564,7 +23564,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -23674,7 +23674,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -23780,7 +23780,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -23890,7 +23890,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -24000,7 +24000,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -24110,7 +24110,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -24224,7 +24224,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -24338,7 +24338,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -24452,7 +24452,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -24562,7 +24562,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -24668,7 +24668,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -24778,7 +24778,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -24880,7 +24880,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -24990,7 +24990,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -25096,7 +25096,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -25202,7 +25202,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -25308,7 +25308,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -25414,7 +25414,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -25524,7 +25524,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -25626,7 +25626,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -25732,7 +25732,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -25842,7 +25842,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -25952,7 +25952,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -26054,7 +26054,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -26164,7 +26164,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -26270,7 +26270,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -26380,7 +26380,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -26486,7 +26486,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -26592,7 +26592,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -26698,7 +26698,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -26804,7 +26804,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -26918,7 +26918,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -27024,7 +27024,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -27134,7 +27134,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -27248,7 +27248,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -27358,7 +27358,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -27468,7 +27468,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -27578,7 +27578,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -27688,7 +27688,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -27794,7 +27794,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -27900,7 +27900,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -28006,7 +28006,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -28112,7 +28112,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -28218,7 +28218,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -28328,7 +28328,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -28442,7 +28442,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -28552,7 +28552,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -28658,7 +28658,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -28772,7 +28772,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -28878,7 +28878,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -28984,7 +28984,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -29098,7 +29098,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -29208,7 +29208,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -29310,7 +29310,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -29416,7 +29416,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -29522,7 +29522,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -29632,7 +29632,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -29738,7 +29738,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -29848,7 +29848,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -29962,7 +29962,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -30064,7 +30064,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -30174,7 +30174,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -30280,7 +30280,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -30390,7 +30390,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -30500,7 +30500,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -30610,7 +30610,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -30716,7 +30716,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -30830,7 +30830,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -30936,7 +30936,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -31046,7 +31046,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -31156,7 +31156,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -31258,7 +31258,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -31364,7 +31364,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -31474,7 +31474,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -31588,7 +31588,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -31694,7 +31694,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -31804,7 +31804,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -31918,7 +31918,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -32028,7 +32028,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -32138,7 +32138,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -32248,7 +32248,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -32354,7 +32354,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -32468,7 +32468,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -32582,7 +32582,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -32696,7 +32696,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -32806,7 +32806,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -32912,7 +32912,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -33022,7 +33022,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -33132,7 +33132,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -33246,7 +33246,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -33352,7 +33352,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -33454,7 +33454,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -33560,7 +33560,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -33670,7 +33670,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -33780,7 +33780,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -33890,7 +33890,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -33996,7 +33996,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -34102,7 +34102,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -34216,7 +34216,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -34322,7 +34322,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -34428,7 +34428,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -34542,7 +34542,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -34656,7 +34656,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -34762,7 +34762,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -34872,7 +34872,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -34986,7 +34986,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -35092,7 +35092,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -35198,7 +35198,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -35308,7 +35308,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -35414,7 +35414,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -35520,7 +35520,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -35626,7 +35626,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -35728,7 +35728,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -35838,7 +35838,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -35940,7 +35940,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -36054,7 +36054,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -36160,7 +36160,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -36266,7 +36266,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -36368,7 +36368,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -36482,7 +36482,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -36596,7 +36596,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -36702,7 +36702,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -36812,7 +36812,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -36914,7 +36914,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -37024,7 +37024,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -37130,7 +37130,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -37232,7 +37232,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -37342,7 +37342,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -37452,7 +37452,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -37562,7 +37562,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -37676,7 +37676,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -37782,7 +37782,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -37892,7 +37892,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -37998,7 +37998,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -38104,7 +38104,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -38218,7 +38218,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -38324,7 +38324,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -38426,7 +38426,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -38540,7 +38540,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -38650,7 +38650,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -38756,7 +38756,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -38870,7 +38870,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -38976,7 +38976,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -39086,7 +39086,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -39196,7 +39196,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -39298,7 +39298,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -39404,7 +39404,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -39518,7 +39518,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -39624,7 +39624,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -39734,7 +39734,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -39840,7 +39840,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -39946,7 +39946,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -40048,7 +40048,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -40150,7 +40150,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -40260,7 +40260,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -40366,7 +40366,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -40476,7 +40476,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -40578,7 +40578,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -40684,7 +40684,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -40790,7 +40790,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -40896,7 +40896,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -40998,7 +40998,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -41100,7 +41100,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -41206,7 +41206,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -41316,7 +41316,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -41422,7 +41422,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -41528,7 +41528,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -41638,7 +41638,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -41748,7 +41748,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -41850,7 +41850,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -41960,7 +41960,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -42062,7 +42062,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -42172,7 +42172,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -42278,7 +42278,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -42392,7 +42392,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -42498,7 +42498,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -42612,7 +42612,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -42718,7 +42718,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -42832,7 +42832,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -42942,7 +42942,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -43044,7 +43044,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -43150,7 +43150,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -43264,7 +43264,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -43370,7 +43370,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -43480,7 +43480,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -43582,7 +43582,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -43684,7 +43684,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -43790,7 +43790,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -43900,7 +43900,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -44006,7 +44006,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -44116,7 +44116,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -44222,7 +44222,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -44328,7 +44328,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -44438,7 +44438,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -44544,7 +44544,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -44646,7 +44646,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -44756,7 +44756,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -44862,7 +44862,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -44968,7 +44968,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -45078,7 +45078,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -45180,7 +45180,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -45286,7 +45286,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -45396,7 +45396,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -45510,7 +45510,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -45620,7 +45620,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -45730,7 +45730,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -45832,7 +45832,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -45934,7 +45934,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -46036,7 +46036,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -46146,7 +46146,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -46252,7 +46252,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -46362,7 +46362,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -46472,7 +46472,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -46586,7 +46586,7 @@
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
@@ -46692,7 +46692,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
@@ -46802,7 +46802,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -46908,7 +46908,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -47014,7 +47014,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -47120,7 +47120,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -47226,7 +47226,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
@@ -47332,7 +47332,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
@@ -47442,7 +47442,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -47556,7 +47556,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
@@ -47662,7 +47662,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
@@ -47768,7 +47768,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
@@ -47874,7 +47874,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -47980,7 +47980,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -48090,7 +48090,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -48200,7 +48200,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -48306,7 +48306,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -48412,7 +48412,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -48518,7 +48518,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -48628,7 +48628,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -48730,7 +48730,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -48832,7 +48832,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -48938,7 +48938,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -49040,7 +49040,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -49150,7 +49150,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -49256,7 +49256,7 @@
       </c>
       <c r="E451" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -49362,7 +49362,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -49464,7 +49464,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -49566,7 +49566,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
@@ -49668,7 +49668,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
@@ -49774,7 +49774,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -49876,7 +49876,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
@@ -49982,7 +49982,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
@@ -50092,7 +50092,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
@@ -50198,7 +50198,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -50312,7 +50312,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
@@ -50418,7 +50418,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -50524,7 +50524,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
@@ -50626,7 +50626,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
@@ -50732,7 +50732,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -50834,7 +50834,7 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
@@ -50944,7 +50944,7 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">

</xml_diff>

<commit_message>
Biplots: highlighting samples with zero values
-highlighted the samples with a zero value for the column oth, the samples that had zero value for a mineral and samples that had zeros for both.
-tried to give each combination of minerals a color, but didn't quite turned out the way i wanted
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -650,7 +650,7 @@
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH2" t="n">
@@ -766,7 +766,7 @@
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH3" t="n">
@@ -882,7 +882,7 @@
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH4" t="n">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH5" t="n">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH6" t="n">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH7" t="n">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH8" t="n">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH9" t="n">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="AG10" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH10" t="n">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH11" t="n">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="AG12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH12" t="n">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="AG13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH13" t="n">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="AG14" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH14" t="n">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="AG15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH15" t="n">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="AG16" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH16" t="n">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="AG17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH17" t="n">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="AG18" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH18" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="AG19" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH19" t="n">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="AG20" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH20" t="n">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="AG21" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH21" t="n">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="AG22" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH22" t="n">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="AG23" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH23" t="n">
@@ -3262,7 +3262,7 @@
       </c>
       <c r="AG24" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH24" t="n">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="AG25" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH25" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="AG26" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH26" t="n">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="AG27" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH27" t="n">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="AG28" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH28" t="n">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="AG29" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH29" t="n">
@@ -3966,7 +3966,7 @@
       </c>
       <c r="AG30" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH30" t="n">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="AG31" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH31" t="n">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="AG32" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH32" t="n">
@@ -4330,7 +4330,7 @@
       </c>
       <c r="AG33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH33" t="n">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="AG34" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH34" t="n">
@@ -4570,7 +4570,7 @@
       </c>
       <c r="AG35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH35" t="n">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="AG36" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH36" t="n">
@@ -4810,7 +4810,7 @@
       </c>
       <c r="AG37" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH37" t="n">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="AG38" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH38" t="n">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="AG39" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH39" t="n">
@@ -5170,7 +5170,7 @@
       </c>
       <c r="AG40" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH40" t="n">
@@ -5286,7 +5286,7 @@
       </c>
       <c r="AG41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH41" t="n">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="AG42" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH42" t="n">
@@ -5526,7 +5526,7 @@
       </c>
       <c r="AG43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH43" t="n">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="AG44" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH44" t="n">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="AG45" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH45" t="n">
@@ -5894,7 +5894,7 @@
       </c>
       <c r="AG46" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH46" t="n">
@@ -6010,7 +6010,7 @@
       </c>
       <c r="AG47" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH47" t="n">
@@ -6130,7 +6130,7 @@
       </c>
       <c r="AG48" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH48" t="n">
@@ -6242,7 +6242,7 @@
       </c>
       <c r="AG49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH49" t="n">
@@ -6362,7 +6362,7 @@
       </c>
       <c r="AG50" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH50" t="n">
@@ -6486,7 +6486,7 @@
       </c>
       <c r="AG51" t="inlineStr">
         <is>
-          <t>MnO   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH51" t="n">
@@ -6602,7 +6602,7 @@
       </c>
       <c r="AG52" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH52" t="n">
@@ -6726,7 +6726,7 @@
       </c>
       <c r="AG53" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH53" t="n">
@@ -6850,7 +6850,7 @@
       </c>
       <c r="AG54" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH54" t="n">
@@ -6966,7 +6966,7 @@
       </c>
       <c r="AG55" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH55" t="n">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="AG56" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH56" t="n">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="AG57" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH57" t="n">
@@ -7326,7 +7326,7 @@
       </c>
       <c r="AG58" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH58" t="n">
@@ -7450,7 +7450,7 @@
       </c>
       <c r="AG59" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH59" t="n">
@@ -7570,7 +7570,7 @@
       </c>
       <c r="AG60" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH60" t="n">
@@ -7694,7 +7694,7 @@
       </c>
       <c r="AG61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> TiO2   </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH61" t="n">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="AG62" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH62" t="n">
@@ -7926,7 +7926,7 @@
       </c>
       <c r="AG63" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH63" t="n">
@@ -8050,7 +8050,7 @@
       </c>
       <c r="AG64" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH64" t="n">
@@ -8166,7 +8166,7 @@
       </c>
       <c r="AG65" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH65" t="n">
@@ -8286,7 +8286,7 @@
       </c>
       <c r="AG66" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH66" t="n">
@@ -8398,7 +8398,7 @@
       </c>
       <c r="AG67" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH67" t="n">
@@ -8514,7 +8514,7 @@
       </c>
       <c r="AG68" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH68" t="n">
@@ -8638,7 +8638,7 @@
       </c>
       <c r="AG69" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH69" t="n">
@@ -8758,7 +8758,7 @@
       </c>
       <c r="AG70" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH70" t="n">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="AG71" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH71" t="n">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="AG72" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH72" t="n">
@@ -9126,7 +9126,7 @@
       </c>
       <c r="AG73" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH73" t="n">
@@ -9242,7 +9242,7 @@
       </c>
       <c r="AG74" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH74" t="n">
@@ -9354,7 +9354,7 @@
       </c>
       <c r="AG75" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH75" t="n">
@@ -9470,7 +9470,7 @@
       </c>
       <c r="AG76" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH76" t="n">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="AG77" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH77" t="n">
@@ -9706,7 +9706,7 @@
       </c>
       <c r="AG78" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH78" t="n">
@@ -9826,7 +9826,7 @@
       </c>
       <c r="AG79" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH79" t="n">
@@ -9950,7 +9950,7 @@
       </c>
       <c r="AG80" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH80" t="n">
@@ -10066,7 +10066,7 @@
       </c>
       <c r="AG81" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH81" t="n">
@@ -10186,7 +10186,7 @@
       </c>
       <c r="AG82" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH82" t="n">
@@ -10306,7 +10306,7 @@
       </c>
       <c r="AG83" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH83" t="n">
@@ -10426,7 +10426,7 @@
       </c>
       <c r="AG84" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH84" t="n">
@@ -10550,7 +10550,7 @@
       </c>
       <c r="AG85" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH85" t="n">
@@ -10674,7 +10674,7 @@
       </c>
       <c r="AG86" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH86" t="n">
@@ -10790,7 +10790,7 @@
       </c>
       <c r="AG87" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH87" t="n">
@@ -10906,7 +10906,7 @@
       </c>
       <c r="AG88" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH88" t="n">
@@ -11018,7 +11018,7 @@
       </c>
       <c r="AG89" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH89" t="n">
@@ -11130,7 +11130,7 @@
       </c>
       <c r="AG90" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH90" t="n">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="AG91" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH91" t="n">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="AG92" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH92" t="n">
@@ -11482,7 +11482,7 @@
       </c>
       <c r="AG93" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH93" t="n">
@@ -11598,7 +11598,7 @@
       </c>
       <c r="AG94" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH94" t="n">
@@ -11718,7 +11718,7 @@
       </c>
       <c r="AG95" t="inlineStr">
         <is>
-          <t>MnO TiO2  P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH95" t="n">
@@ -11834,7 +11834,7 @@
       </c>
       <c r="AG96" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH96" t="n">
@@ -11958,7 +11958,7 @@
       </c>
       <c r="AG97" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH97" t="n">
@@ -12082,7 +12082,7 @@
       </c>
       <c r="AG98" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH98" t="n">
@@ -12198,7 +12198,7 @@
       </c>
       <c r="AG99" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH99" t="n">
@@ -12322,7 +12322,7 @@
       </c>
       <c r="AG100" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH100" t="n">
@@ -12446,7 +12446,7 @@
       </c>
       <c r="AG101" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH101" t="n">
@@ -12570,7 +12570,7 @@
       </c>
       <c r="AG102" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH102" t="n">
@@ -12686,7 +12686,7 @@
       </c>
       <c r="AG103" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH103" t="n">
@@ -12806,7 +12806,7 @@
       </c>
       <c r="AG104" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH104" t="n">
@@ -12922,7 +12922,7 @@
       </c>
       <c r="AG105" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH105" t="n">
@@ -13042,7 +13042,7 @@
       </c>
       <c r="AG106" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH106" t="n">
@@ -13162,7 +13162,7 @@
       </c>
       <c r="AG107" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH107" t="n">
@@ -13286,7 +13286,7 @@
       </c>
       <c r="AG108" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH108" t="n">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="AG109" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH109" t="n">
@@ -13522,7 +13522,7 @@
       </c>
       <c r="AG110" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH110" t="n">
@@ -13634,7 +13634,7 @@
       </c>
       <c r="AG111" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH111" t="n">
@@ -13754,7 +13754,7 @@
       </c>
       <c r="AG112" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH112" t="n">
@@ -13870,7 +13870,7 @@
       </c>
       <c r="AG113" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH113" t="n">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="AG114" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH114" t="n">
@@ -14114,7 +14114,7 @@
       </c>
       <c r="AG115" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH115" t="n">
@@ -14238,7 +14238,7 @@
       </c>
       <c r="AG116" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH116" t="n">
@@ -14358,7 +14358,7 @@
       </c>
       <c r="AG117" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH117" t="n">
@@ -14478,7 +14478,7 @@
       </c>
       <c r="AG118" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH118" t="n">
@@ -14598,7 +14598,7 @@
       </c>
       <c r="AG119" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH119" t="n">
@@ -14714,7 +14714,7 @@
       </c>
       <c r="AG120" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH120" t="n">
@@ -14838,7 +14838,7 @@
       </c>
       <c r="AG121" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH121" t="n">
@@ -14962,7 +14962,7 @@
       </c>
       <c r="AG122" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH122" t="n">
@@ -15086,7 +15086,7 @@
       </c>
       <c r="AG123" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH123" t="n">
@@ -15202,7 +15202,7 @@
       </c>
       <c r="AG124" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH124" t="n">
@@ -15318,7 +15318,7 @@
       </c>
       <c r="AG125" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH125" t="n">
@@ -15430,7 +15430,7 @@
       </c>
       <c r="AG126" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH126" t="n">
@@ -15550,7 +15550,7 @@
       </c>
       <c r="AG127" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH127" t="n">
@@ -15662,7 +15662,7 @@
       </c>
       <c r="AG128" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH128" t="n">
@@ -15786,7 +15786,7 @@
       </c>
       <c r="AG129" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH129" t="n">
@@ -15910,7 +15910,7 @@
       </c>
       <c r="AG130" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH130" t="n">
@@ -16026,7 +16026,7 @@
       </c>
       <c r="AG131" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH131" t="n">
@@ -16146,7 +16146,7 @@
       </c>
       <c r="AG132" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH132" t="n">
@@ -16262,7 +16262,7 @@
       </c>
       <c r="AG133" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH133" t="n">
@@ -16374,7 +16374,7 @@
       </c>
       <c r="AG134" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH134" t="n">
@@ -16498,7 +16498,7 @@
       </c>
       <c r="AG135" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH135" t="n">
@@ -16614,7 +16614,7 @@
       </c>
       <c r="AG136" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH136" t="n">
@@ -16734,7 +16734,7 @@
       </c>
       <c r="AG137" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH137" t="n">
@@ -16854,7 +16854,7 @@
       </c>
       <c r="AG138" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH138" t="n">
@@ -16966,7 +16966,7 @@
       </c>
       <c r="AG139" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH139" t="n">
@@ -17090,7 +17090,7 @@
       </c>
       <c r="AG140" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH140" t="n">
@@ -17210,7 +17210,7 @@
       </c>
       <c r="AG141" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH141" t="n">
@@ -17326,7 +17326,7 @@
       </c>
       <c r="AG142" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH142" t="n">
@@ -17450,7 +17450,7 @@
       </c>
       <c r="AG143" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH143" t="n">
@@ -17570,7 +17570,7 @@
       </c>
       <c r="AG144" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH144" t="n">
@@ -17686,7 +17686,7 @@
       </c>
       <c r="AG145" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH145" t="n">
@@ -17802,7 +17802,7 @@
       </c>
       <c r="AG146" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH146" t="n">
@@ -17918,7 +17918,7 @@
       </c>
       <c r="AG147" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH147" t="n">
@@ -18034,7 +18034,7 @@
       </c>
       <c r="AG148" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH148" t="n">
@@ -18150,7 +18150,7 @@
       </c>
       <c r="AG149" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH149" t="n">
@@ -18274,7 +18274,7 @@
       </c>
       <c r="AG150" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH150" t="n">
@@ -18398,7 +18398,7 @@
       </c>
       <c r="AG151" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH151" t="n">
@@ -18522,7 +18522,7 @@
       </c>
       <c r="AG152" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH152" t="n">
@@ -18642,7 +18642,7 @@
       </c>
       <c r="AG153" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH153" t="n">
@@ -18758,7 +18758,7 @@
       </c>
       <c r="AG154" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH154" t="n">
@@ -18878,7 +18878,7 @@
       </c>
       <c r="AG155" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH155" t="n">
@@ -19002,7 +19002,7 @@
       </c>
       <c r="AG156" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH156" t="n">
@@ -19122,7 +19122,7 @@
       </c>
       <c r="AG157" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH157" t="n">
@@ -19238,7 +19238,7 @@
       </c>
       <c r="AG158" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH158" t="n">
@@ -19350,7 +19350,7 @@
       </c>
       <c r="AG159" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH159" t="n">
@@ -19474,7 +19474,7 @@
       </c>
       <c r="AG160" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH160" t="n">
@@ -19594,7 +19594,7 @@
       </c>
       <c r="AG161" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH161" t="n">
@@ -19718,7 +19718,7 @@
       </c>
       <c r="AG162" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH162" t="n">
@@ -19842,7 +19842,7 @@
       </c>
       <c r="AG163" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH163" t="n">
@@ -19962,7 +19962,7 @@
       </c>
       <c r="AG164" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH164" t="n">
@@ -20078,7 +20078,7 @@
       </c>
       <c r="AG165" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH165" t="n">
@@ -20198,7 +20198,7 @@
       </c>
       <c r="AG166" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH166" t="n">
@@ -20314,7 +20314,7 @@
       </c>
       <c r="AG167" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH167" t="n">
@@ -20430,7 +20430,7 @@
       </c>
       <c r="AG168" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH168" t="n">
@@ -20546,7 +20546,7 @@
       </c>
       <c r="AG169" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH169" t="n">
@@ -20666,7 +20666,7 @@
       </c>
       <c r="AG170" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH170" t="n">
@@ -20790,7 +20790,7 @@
       </c>
       <c r="AG171" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH171" t="n">
@@ -20906,7 +20906,7 @@
       </c>
       <c r="AG172" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH172" t="n">
@@ -21026,7 +21026,7 @@
       </c>
       <c r="AG173" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH173" t="n">
@@ -21150,7 +21150,7 @@
       </c>
       <c r="AG174" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH174" t="n">
@@ -21270,7 +21270,7 @@
       </c>
       <c r="AG175" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH175" t="n">
@@ -21390,7 +21390,7 @@
       </c>
       <c r="AG176" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH176" t="n">
@@ -21510,7 +21510,7 @@
       </c>
       <c r="AG177" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH177" t="n">
@@ -21626,7 +21626,7 @@
       </c>
       <c r="AG178" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH178" t="n">
@@ -21746,7 +21746,7 @@
       </c>
       <c r="AG179" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH179" t="n">
@@ -21866,7 +21866,7 @@
       </c>
       <c r="AG180" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH180" t="n">
@@ -21982,7 +21982,7 @@
       </c>
       <c r="AG181" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH181" t="n">
@@ -22102,7 +22102,7 @@
       </c>
       <c r="AG182" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH182" t="n">
@@ -22218,7 +22218,7 @@
       </c>
       <c r="AG183" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH183" t="n">
@@ -22334,7 +22334,7 @@
       </c>
       <c r="AG184" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH184" t="n">
@@ -22458,7 +22458,7 @@
       </c>
       <c r="AG185" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH185" t="n">
@@ -22578,7 +22578,7 @@
       </c>
       <c r="AG186" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH186" t="n">
@@ -22702,7 +22702,7 @@
       </c>
       <c r="AG187" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH187" t="n">
@@ -22822,7 +22822,7 @@
       </c>
       <c r="AG188" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH188" t="n">
@@ -22942,7 +22942,7 @@
       </c>
       <c r="AG189" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH189" t="n">
@@ -23058,7 +23058,7 @@
       </c>
       <c r="AG190" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH190" t="n">
@@ -23178,7 +23178,7 @@
       </c>
       <c r="AG191" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH191" t="n">
@@ -23302,7 +23302,7 @@
       </c>
       <c r="AG192" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH192" t="n">
@@ -23422,7 +23422,7 @@
       </c>
       <c r="AG193" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH193" t="n">
@@ -23542,7 +23542,7 @@
       </c>
       <c r="AG194" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH194" t="n">
@@ -23662,7 +23662,7 @@
       </c>
       <c r="AG195" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH195" t="n">
@@ -23782,7 +23782,7 @@
       </c>
       <c r="AG196" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH196" t="n">
@@ -23894,7 +23894,7 @@
       </c>
       <c r="AG197" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH197" t="n">
@@ -24010,7 +24010,7 @@
       </c>
       <c r="AG198" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH198" t="n">
@@ -24134,7 +24134,7 @@
       </c>
       <c r="AG199" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH199" t="n">
@@ -24254,7 +24254,7 @@
       </c>
       <c r="AG200" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH200" t="n">
@@ -24374,7 +24374,7 @@
       </c>
       <c r="AG201" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH201" t="n">
@@ -24490,7 +24490,7 @@
       </c>
       <c r="AG202" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH202" t="n">
@@ -24606,7 +24606,7 @@
       </c>
       <c r="AG203" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH203" t="n">
@@ -24726,7 +24726,7 @@
       </c>
       <c r="AG204" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH204" t="n">
@@ -24838,7 +24838,7 @@
       </c>
       <c r="AG205" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH205" t="n">
@@ -24954,7 +24954,7 @@
       </c>
       <c r="AG206" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH206" t="n">
@@ -25070,7 +25070,7 @@
       </c>
       <c r="AG207" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH207" t="n">
@@ -25190,7 +25190,7 @@
       </c>
       <c r="AG208" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH208" t="n">
@@ -25306,7 +25306,7 @@
       </c>
       <c r="AG209" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH209" t="n">
@@ -25426,7 +25426,7 @@
       </c>
       <c r="AG210" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH210" t="n">
@@ -25542,7 +25542,7 @@
       </c>
       <c r="AG211" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH211" t="n">
@@ -25662,7 +25662,7 @@
       </c>
       <c r="AG212" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH212" t="n">
@@ -25782,7 +25782,7 @@
       </c>
       <c r="AG213" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH213" t="n">
@@ -25898,7 +25898,7 @@
       </c>
       <c r="AG214" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH214" t="n">
@@ -26018,7 +26018,7 @@
       </c>
       <c r="AG215" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH215" t="n">
@@ -26138,7 +26138,7 @@
       </c>
       <c r="AG216" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH216" t="n">
@@ -26258,7 +26258,7 @@
       </c>
       <c r="AG217" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH217" t="n">
@@ -26382,7 +26382,7 @@
       </c>
       <c r="AG218" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH218" t="n">
@@ -26506,7 +26506,7 @@
       </c>
       <c r="AG219" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH219" t="n">
@@ -26630,7 +26630,7 @@
       </c>
       <c r="AG220" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH220" t="n">
@@ -26750,7 +26750,7 @@
       </c>
       <c r="AG221" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH221" t="n">
@@ -26866,7 +26866,7 @@
       </c>
       <c r="AG222" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH222" t="n">
@@ -26986,7 +26986,7 @@
       </c>
       <c r="AG223" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH223" t="n">
@@ -27098,7 +27098,7 @@
       </c>
       <c r="AG224" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH224" t="n">
@@ -27218,7 +27218,7 @@
       </c>
       <c r="AG225" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH225" t="n">
@@ -27334,7 +27334,7 @@
       </c>
       <c r="AG226" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH226" t="n">
@@ -27450,7 +27450,7 @@
       </c>
       <c r="AG227" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH227" t="n">
@@ -27566,7 +27566,7 @@
       </c>
       <c r="AG228" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH228" t="n">
@@ -27682,7 +27682,7 @@
       </c>
       <c r="AG229" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH229" t="n">
@@ -27802,7 +27802,7 @@
       </c>
       <c r="AG230" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH230" t="n">
@@ -27914,7 +27914,7 @@
       </c>
       <c r="AG231" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH231" t="n">
@@ -28030,7 +28030,7 @@
       </c>
       <c r="AG232" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH232" t="n">
@@ -28150,7 +28150,7 @@
       </c>
       <c r="AG233" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH233" t="n">
@@ -28270,7 +28270,7 @@
       </c>
       <c r="AG234" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH234" t="n">
@@ -28382,7 +28382,7 @@
       </c>
       <c r="AG235" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH235" t="n">
@@ -28502,7 +28502,7 @@
       </c>
       <c r="AG236" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH236" t="n">
@@ -28618,7 +28618,7 @@
       </c>
       <c r="AG237" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH237" t="n">
@@ -28738,7 +28738,7 @@
       </c>
       <c r="AG238" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH238" t="n">
@@ -28854,7 +28854,7 @@
       </c>
       <c r="AG239" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH239" t="n">
@@ -28970,7 +28970,7 @@
       </c>
       <c r="AG240" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH240" t="n">
@@ -29086,7 +29086,7 @@
       </c>
       <c r="AG241" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH241" t="n">
@@ -29202,7 +29202,7 @@
       </c>
       <c r="AG242" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH242" t="n">
@@ -29326,7 +29326,7 @@
       </c>
       <c r="AG243" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH243" t="n">
@@ -29442,7 +29442,7 @@
       </c>
       <c r="AG244" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH244" t="n">
@@ -29562,7 +29562,7 @@
       </c>
       <c r="AG245" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH245" t="n">
@@ -29686,7 +29686,7 @@
       </c>
       <c r="AG246" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH246" t="n">
@@ -29806,7 +29806,7 @@
       </c>
       <c r="AG247" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH247" t="n">
@@ -29926,7 +29926,7 @@
       </c>
       <c r="AG248" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH248" t="n">
@@ -30046,7 +30046,7 @@
       </c>
       <c r="AG249" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH249" t="n">
@@ -30166,7 +30166,7 @@
       </c>
       <c r="AG250" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH250" t="n">
@@ -30282,7 +30282,7 @@
       </c>
       <c r="AG251" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH251" t="n">
@@ -30398,7 +30398,7 @@
       </c>
       <c r="AG252" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH252" t="n">
@@ -30514,7 +30514,7 @@
       </c>
       <c r="AG253" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH253" t="n">
@@ -30630,7 +30630,7 @@
       </c>
       <c r="AG254" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH254" t="n">
@@ -30746,7 +30746,7 @@
       </c>
       <c r="AG255" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH255" t="n">
@@ -30866,7 +30866,7 @@
       </c>
       <c r="AG256" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH256" t="n">
@@ -30990,7 +30990,7 @@
       </c>
       <c r="AG257" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH257" t="n">
@@ -31110,7 +31110,7 @@
       </c>
       <c r="AG258" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH258" t="n">
@@ -31226,7 +31226,7 @@
       </c>
       <c r="AG259" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH259" t="n">
@@ -31350,7 +31350,7 @@
       </c>
       <c r="AG260" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH260" t="n">
@@ -31466,7 +31466,7 @@
       </c>
       <c r="AG261" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH261" t="n">
@@ -31582,7 +31582,7 @@
       </c>
       <c r="AG262" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH262" t="n">
@@ -31706,7 +31706,7 @@
       </c>
       <c r="AG263" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH263" t="n">
@@ -31826,7 +31826,7 @@
       </c>
       <c r="AG264" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH264" t="n">
@@ -31938,7 +31938,7 @@
       </c>
       <c r="AG265" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH265" t="n">
@@ -32054,7 +32054,7 @@
       </c>
       <c r="AG266" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH266" t="n">
@@ -32170,7 +32170,7 @@
       </c>
       <c r="AG267" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH267" t="n">
@@ -32290,7 +32290,7 @@
       </c>
       <c r="AG268" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH268" t="n">
@@ -32406,7 +32406,7 @@
       </c>
       <c r="AG269" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH269" t="n">
@@ -32526,7 +32526,7 @@
       </c>
       <c r="AG270" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH270" t="n">
@@ -32650,7 +32650,7 @@
       </c>
       <c r="AG271" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH271" t="n">
@@ -32762,7 +32762,7 @@
       </c>
       <c r="AG272" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH272" t="n">
@@ -32882,7 +32882,7 @@
       </c>
       <c r="AG273" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH273" t="n">
@@ -32998,7 +32998,7 @@
       </c>
       <c r="AG274" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH274" t="n">
@@ -33118,7 +33118,7 @@
       </c>
       <c r="AG275" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH275" t="n">
@@ -33238,7 +33238,7 @@
       </c>
       <c r="AG276" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH276" t="n">
@@ -33358,7 +33358,7 @@
       </c>
       <c r="AG277" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH277" t="n">
@@ -33474,7 +33474,7 @@
       </c>
       <c r="AG278" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH278" t="n">
@@ -33598,7 +33598,7 @@
       </c>
       <c r="AG279" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH279" t="n">
@@ -33714,7 +33714,7 @@
       </c>
       <c r="AG280" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH280" t="n">
@@ -33834,7 +33834,7 @@
       </c>
       <c r="AG281" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH281" t="n">
@@ -33954,7 +33954,7 @@
       </c>
       <c r="AG282" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH282" t="n">
@@ -34066,7 +34066,7 @@
       </c>
       <c r="AG283" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH283" t="n">
@@ -34182,7 +34182,7 @@
       </c>
       <c r="AG284" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH284" t="n">
@@ -34302,7 +34302,7 @@
       </c>
       <c r="AG285" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH285" t="n">
@@ -34426,7 +34426,7 @@
       </c>
       <c r="AG286" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH286" t="n">
@@ -34542,7 +34542,7 @@
       </c>
       <c r="AG287" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH287" t="n">
@@ -34662,7 +34662,7 @@
       </c>
       <c r="AG288" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH288" t="n">
@@ -34786,7 +34786,7 @@
       </c>
       <c r="AG289" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH289" t="n">
@@ -34906,7 +34906,7 @@
       </c>
       <c r="AG290" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH290" t="n">
@@ -35026,7 +35026,7 @@
       </c>
       <c r="AG291" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH291" t="n">
@@ -35146,7 +35146,7 @@
       </c>
       <c r="AG292" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH292" t="n">
@@ -35262,7 +35262,7 @@
       </c>
       <c r="AG293" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH293" t="n">
@@ -35386,7 +35386,7 @@
       </c>
       <c r="AG294" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH294" t="n">
@@ -35510,7 +35510,7 @@
       </c>
       <c r="AG295" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH295" t="n">
@@ -35634,7 +35634,7 @@
       </c>
       <c r="AG296" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH296" t="n">
@@ -35754,7 +35754,7 @@
       </c>
       <c r="AG297" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH297" t="n">
@@ -35870,7 +35870,7 @@
       </c>
       <c r="AG298" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH298" t="n">
@@ -35990,7 +35990,7 @@
       </c>
       <c r="AG299" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH299" t="n">
@@ -36110,7 +36110,7 @@
       </c>
       <c r="AG300" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH300" t="n">
@@ -36234,7 +36234,7 @@
       </c>
       <c r="AG301" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH301" t="n">
@@ -36350,7 +36350,7 @@
       </c>
       <c r="AG302" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH302" t="n">
@@ -36462,7 +36462,7 @@
       </c>
       <c r="AG303" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH303" t="n">
@@ -36578,7 +36578,7 @@
       </c>
       <c r="AG304" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH304" t="n">
@@ -36698,7 +36698,7 @@
       </c>
       <c r="AG305" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH305" t="n">
@@ -36818,7 +36818,7 @@
       </c>
       <c r="AG306" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH306" t="n">
@@ -36938,7 +36938,7 @@
       </c>
       <c r="AG307" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH307" t="n">
@@ -37054,7 +37054,7 @@
       </c>
       <c r="AG308" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH308" t="n">
@@ -37170,7 +37170,7 @@
       </c>
       <c r="AG309" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH309" t="n">
@@ -37294,7 +37294,7 @@
       </c>
       <c r="AG310" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH310" t="n">
@@ -37410,7 +37410,7 @@
       </c>
       <c r="AG311" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH311" t="n">
@@ -37526,7 +37526,7 @@
       </c>
       <c r="AG312" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH312" t="n">
@@ -37650,7 +37650,7 @@
       </c>
       <c r="AG313" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH313" t="n">
@@ -37774,7 +37774,7 @@
       </c>
       <c r="AG314" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH314" t="n">
@@ -37890,7 +37890,7 @@
       </c>
       <c r="AG315" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH315" t="n">
@@ -38010,7 +38010,7 @@
       </c>
       <c r="AG316" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH316" t="n">
@@ -38134,7 +38134,7 @@
       </c>
       <c r="AG317" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH317" t="n">
@@ -38250,7 +38250,7 @@
       </c>
       <c r="AG318" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH318" t="n">
@@ -38366,7 +38366,7 @@
       </c>
       <c r="AG319" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH319" t="n">
@@ -38486,7 +38486,7 @@
       </c>
       <c r="AG320" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH320" t="n">
@@ -38602,7 +38602,7 @@
       </c>
       <c r="AG321" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH321" t="n">
@@ -38718,7 +38718,7 @@
       </c>
       <c r="AG322" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH322" t="n">
@@ -38834,7 +38834,7 @@
       </c>
       <c r="AG323" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH323" t="n">
@@ -38946,7 +38946,7 @@
       </c>
       <c r="AG324" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH324" t="n">
@@ -39066,7 +39066,7 @@
       </c>
       <c r="AG325" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH325" t="n">
@@ -39178,7 +39178,7 @@
       </c>
       <c r="AG326" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH326" t="n">
@@ -39302,7 +39302,7 @@
       </c>
       <c r="AG327" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH327" t="n">
@@ -39418,7 +39418,7 @@
       </c>
       <c r="AG328" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH328" t="n">
@@ -39534,7 +39534,7 @@
       </c>
       <c r="AG329" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH329" t="n">
@@ -39646,7 +39646,7 @@
       </c>
       <c r="AG330" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH330" t="n">
@@ -39770,7 +39770,7 @@
       </c>
       <c r="AG331" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH331" t="n">
@@ -39894,7 +39894,7 @@
       </c>
       <c r="AG332" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH332" t="n">
@@ -40010,7 +40010,7 @@
       </c>
       <c r="AG333" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH333" t="n">
@@ -40130,7 +40130,7 @@
       </c>
       <c r="AG334" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH334" t="n">
@@ -40242,7 +40242,7 @@
       </c>
       <c r="AG335" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH335" t="n">
@@ -40362,7 +40362,7 @@
       </c>
       <c r="AG336" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH336" t="n">
@@ -40478,7 +40478,7 @@
       </c>
       <c r="AG337" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH337" t="n">
@@ -40590,7 +40590,7 @@
       </c>
       <c r="AG338" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH338" t="n">
@@ -40710,7 +40710,7 @@
       </c>
       <c r="AG339" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH339" t="n">
@@ -40830,7 +40830,7 @@
       </c>
       <c r="AG340" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH340" t="n">
@@ -40950,7 +40950,7 @@
       </c>
       <c r="AG341" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH341" t="n">
@@ -41074,7 +41074,7 @@
       </c>
       <c r="AG342" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH342" t="n">
@@ -41190,7 +41190,7 @@
       </c>
       <c r="AG343" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH343" t="n">
@@ -41310,7 +41310,7 @@
       </c>
       <c r="AG344" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH344" t="n">
@@ -41426,7 +41426,7 @@
       </c>
       <c r="AG345" t="inlineStr">
         <is>
-          <t>MnO   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH345" t="n">
@@ -41542,7 +41542,7 @@
       </c>
       <c r="AG346" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH346" t="n">
@@ -41666,7 +41666,7 @@
       </c>
       <c r="AG347" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH347" t="n">
@@ -41782,7 +41782,7 @@
       </c>
       <c r="AG348" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH348" t="n">
@@ -41894,7 +41894,7 @@
       </c>
       <c r="AG349" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH349" t="n">
@@ -42018,7 +42018,7 @@
       </c>
       <c r="AG350" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH350" t="n">
@@ -42138,7 +42138,7 @@
       </c>
       <c r="AG351" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH351" t="n">
@@ -42254,7 +42254,7 @@
       </c>
       <c r="AG352" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH352" t="n">
@@ -42378,7 +42378,7 @@
       </c>
       <c r="AG353" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH353" t="n">
@@ -42494,7 +42494,7 @@
       </c>
       <c r="AG354" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH354" t="n">
@@ -42614,7 +42614,7 @@
       </c>
       <c r="AG355" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH355" t="n">
@@ -42734,7 +42734,7 @@
       </c>
       <c r="AG356" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH356" t="n">
@@ -42846,7 +42846,7 @@
       </c>
       <c r="AG357" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH357" t="n">
@@ -42962,7 +42962,7 @@
       </c>
       <c r="AG358" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH358" t="n">
@@ -43086,7 +43086,7 @@
       </c>
       <c r="AG359" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH359" t="n">
@@ -43202,7 +43202,7 @@
       </c>
       <c r="AG360" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH360" t="n">
@@ -43322,7 +43322,7 @@
       </c>
       <c r="AG361" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH361" t="n">
@@ -43438,7 +43438,7 @@
       </c>
       <c r="AG362" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH362" t="n">
@@ -43554,7 +43554,7 @@
       </c>
       <c r="AG363" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH363" t="n">
@@ -43666,7 +43666,7 @@
       </c>
       <c r="AG364" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH364" t="n">
@@ -43778,7 +43778,7 @@
       </c>
       <c r="AG365" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH365" t="n">
@@ -43898,7 +43898,7 @@
       </c>
       <c r="AG366" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH366" t="n">
@@ -44014,7 +44014,7 @@
       </c>
       <c r="AG367" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH367" t="n">
@@ -44134,7 +44134,7 @@
       </c>
       <c r="AG368" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH368" t="n">
@@ -44246,7 +44246,7 @@
       </c>
       <c r="AG369" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH369" t="n">
@@ -44362,7 +44362,7 @@
       </c>
       <c r="AG370" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH370" t="n">
@@ -44478,7 +44478,7 @@
       </c>
       <c r="AG371" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH371" t="n">
@@ -44594,7 +44594,7 @@
       </c>
       <c r="AG372" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH372" t="n">
@@ -44706,7 +44706,7 @@
       </c>
       <c r="AG373" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH373" t="n">
@@ -44818,7 +44818,7 @@
       </c>
       <c r="AG374" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH374" t="n">
@@ -44934,7 +44934,7 @@
       </c>
       <c r="AG375" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH375" t="n">
@@ -45054,7 +45054,7 @@
       </c>
       <c r="AG376" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH376" t="n">
@@ -45170,7 +45170,7 @@
       </c>
       <c r="AG377" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH377" t="n">
@@ -45286,7 +45286,7 @@
       </c>
       <c r="AG378" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH378" t="n">
@@ -45406,7 +45406,7 @@
       </c>
       <c r="AG379" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH379" t="n">
@@ -45526,7 +45526,7 @@
       </c>
       <c r="AG380" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH380" t="n">
@@ -45638,7 +45638,7 @@
       </c>
       <c r="AG381" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH381" t="n">
@@ -45758,7 +45758,7 @@
       </c>
       <c r="AG382" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH382" t="n">
@@ -45870,7 +45870,7 @@
       </c>
       <c r="AG383" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH383" t="n">
@@ -45990,7 +45990,7 @@
       </c>
       <c r="AG384" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH384" t="n">
@@ -46106,7 +46106,7 @@
       </c>
       <c r="AG385" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH385" t="n">
@@ -46230,7 +46230,7 @@
       </c>
       <c r="AG386" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH386" t="n">
@@ -46346,7 +46346,7 @@
       </c>
       <c r="AG387" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH387" t="n">
@@ -46470,7 +46470,7 @@
       </c>
       <c r="AG388" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH388" t="n">
@@ -46586,7 +46586,7 @@
       </c>
       <c r="AG389" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH389" t="n">
@@ -46710,7 +46710,7 @@
       </c>
       <c r="AG390" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH390" t="n">
@@ -46830,7 +46830,7 @@
       </c>
       <c r="AG391" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH391" t="n">
@@ -46942,7 +46942,7 @@
       </c>
       <c r="AG392" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH392" t="n">
@@ -47058,7 +47058,7 @@
       </c>
       <c r="AG393" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH393" t="n">
@@ -47182,7 +47182,7 @@
       </c>
       <c r="AG394" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH394" t="n">
@@ -47298,7 +47298,7 @@
       </c>
       <c r="AG395" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH395" t="n">
@@ -47418,7 +47418,7 @@
       </c>
       <c r="AG396" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH396" t="n">
@@ -47530,7 +47530,7 @@
       </c>
       <c r="AG397" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH397" t="n">
@@ -47642,7 +47642,7 @@
       </c>
       <c r="AG398" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH398" t="n">
@@ -47758,7 +47758,7 @@
       </c>
       <c r="AG399" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH399" t="n">
@@ -47878,7 +47878,7 @@
       </c>
       <c r="AG400" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH400" t="n">
@@ -47994,7 +47994,7 @@
       </c>
       <c r="AG401" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH401" t="n">
@@ -48114,7 +48114,7 @@
       </c>
       <c r="AG402" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH402" t="n">
@@ -48230,7 +48230,7 @@
       </c>
       <c r="AG403" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH403" t="n">
@@ -48346,7 +48346,7 @@
       </c>
       <c r="AG404" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH404" t="n">
@@ -48466,7 +48466,7 @@
       </c>
       <c r="AG405" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH405" t="n">
@@ -48582,7 +48582,7 @@
       </c>
       <c r="AG406" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH406" t="n">
@@ -48694,7 +48694,7 @@
       </c>
       <c r="AG407" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH407" t="n">
@@ -48814,7 +48814,7 @@
       </c>
       <c r="AG408" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH408" t="n">
@@ -48930,7 +48930,7 @@
       </c>
       <c r="AG409" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH409" t="n">
@@ -49046,7 +49046,7 @@
       </c>
       <c r="AG410" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH410" t="n">
@@ -49166,7 +49166,7 @@
       </c>
       <c r="AG411" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH411" t="n">
@@ -49278,7 +49278,7 @@
       </c>
       <c r="AG412" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH412" t="n">
@@ -49394,7 +49394,7 @@
       </c>
       <c r="AG413" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH413" t="n">
@@ -49514,7 +49514,7 @@
       </c>
       <c r="AG414" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH414" t="n">
@@ -49638,7 +49638,7 @@
       </c>
       <c r="AG415" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH415" t="n">
@@ -49758,7 +49758,7 @@
       </c>
       <c r="AG416" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH416" t="n">
@@ -49878,7 +49878,7 @@
       </c>
       <c r="AG417" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH417" t="n">
@@ -49990,7 +49990,7 @@
       </c>
       <c r="AG418" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH418" t="n">
@@ -50102,7 +50102,7 @@
       </c>
       <c r="AG419" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH419" t="n">
@@ -50214,7 +50214,7 @@
       </c>
       <c r="AG420" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH420" t="n">
@@ -50334,7 +50334,7 @@
       </c>
       <c r="AG421" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH421" t="n">
@@ -50450,7 +50450,7 @@
       </c>
       <c r="AG422" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH422" t="n">
@@ -50570,7 +50570,7 @@
       </c>
       <c r="AG423" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH423" t="n">
@@ -50690,7 +50690,7 @@
       </c>
       <c r="AG424" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH424" t="n">
@@ -50814,7 +50814,7 @@
       </c>
       <c r="AG425" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH425" t="n">
@@ -50930,7 +50930,7 @@
       </c>
       <c r="AG426" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH426" t="n">
@@ -51050,7 +51050,7 @@
       </c>
       <c r="AG427" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH427" t="n">
@@ -51166,7 +51166,7 @@
       </c>
       <c r="AG428" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH428" t="n">
@@ -51282,7 +51282,7 @@
       </c>
       <c r="AG429" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH429" t="n">
@@ -51398,7 +51398,7 @@
       </c>
       <c r="AG430" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH430" t="n">
@@ -51514,7 +51514,7 @@
       </c>
       <c r="AG431" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH431" t="n">
@@ -51630,7 +51630,7 @@
       </c>
       <c r="AG432" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH432" t="n">
@@ -51750,7 +51750,7 @@
       </c>
       <c r="AG433" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH433" t="n">
@@ -51874,7 +51874,7 @@
       </c>
       <c r="AG434" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH434" t="n">
@@ -51990,7 +51990,7 @@
       </c>
       <c r="AG435" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH435" t="n">
@@ -52106,7 +52106,7 @@
       </c>
       <c r="AG436" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH436" t="n">
@@ -52222,7 +52222,7 @@
       </c>
       <c r="AG437" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH437" t="n">
@@ -52338,7 +52338,7 @@
       </c>
       <c r="AG438" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH438" t="n">
@@ -52458,7 +52458,7 @@
       </c>
       <c r="AG439" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH439" t="n">
@@ -52578,7 +52578,7 @@
       </c>
       <c r="AG440" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH440" t="n">
@@ -52694,7 +52694,7 @@
       </c>
       <c r="AG441" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH441" t="n">
@@ -52810,7 +52810,7 @@
       </c>
       <c r="AG442" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH442" t="n">
@@ -52926,7 +52926,7 @@
       </c>
       <c r="AG443" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH443" t="n">
@@ -53046,7 +53046,7 @@
       </c>
       <c r="AG444" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH444" t="n">
@@ -53158,7 +53158,7 @@
       </c>
       <c r="AG445" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH445" t="n">
@@ -53270,7 +53270,7 @@
       </c>
       <c r="AG446" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH446" t="n">
@@ -53386,7 +53386,7 @@
       </c>
       <c r="AG447" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH447" t="n">
@@ -53498,7 +53498,7 @@
       </c>
       <c r="AG448" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH448" t="n">
@@ -53618,7 +53618,7 @@
       </c>
       <c r="AG449" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH449" t="n">
@@ -53734,7 +53734,7 @@
       </c>
       <c r="AG450" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH450" t="n">
@@ -53850,7 +53850,7 @@
       </c>
       <c r="AG451" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH451" t="n">
@@ -53962,7 +53962,7 @@
       </c>
       <c r="AG452" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH452" t="n">
@@ -54074,7 +54074,7 @@
       </c>
       <c r="AG453" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 oth</t>
+          <t>mineraloth</t>
         </is>
       </c>
       <c r="AH453" t="n">
@@ -54186,7 +54186,7 @@
       </c>
       <c r="AG454" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH454" t="n">
@@ -54302,7 +54302,7 @@
       </c>
       <c r="AG455" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH455" t="n">
@@ -54414,7 +54414,7 @@
       </c>
       <c r="AG456" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH456" t="n">
@@ -54530,7 +54530,7 @@
       </c>
       <c r="AG457" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH457" t="n">
@@ -54650,7 +54650,7 @@
       </c>
       <c r="AG458" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH458" t="n">
@@ -54766,7 +54766,7 @@
       </c>
       <c r="AG459" t="inlineStr">
         <is>
-          <t xml:space="preserve">    </t>
+          <t>no_zero</t>
         </is>
       </c>
       <c r="AH459" t="n">
@@ -54890,7 +54890,7 @@
       </c>
       <c r="AG460" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH460" t="n">
@@ -55006,7 +55006,7 @@
       </c>
       <c r="AG461" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH461" t="n">
@@ -55122,7 +55122,7 @@
       </c>
       <c r="AG462" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH462" t="n">
@@ -55234,7 +55234,7 @@
       </c>
       <c r="AG463" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH463" t="n">
@@ -55350,7 +55350,7 @@
       </c>
       <c r="AG464" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH464" t="n">
@@ -55462,7 +55462,7 @@
       </c>
       <c r="AG465" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH465" t="n">
@@ -55582,7 +55582,7 @@
       </c>
       <c r="AG466" t="inlineStr">
         <is>
-          <t xml:space="preserve">    oth</t>
+          <t>oth</t>
         </is>
       </c>
       <c r="AH466" t="n">
@@ -55706,7 +55706,7 @@
       </c>
       <c r="AG467" t="inlineStr">
         <is>
-          <t xml:space="preserve">   P2O5 </t>
+          <t>mineral</t>
         </is>
       </c>
       <c r="AH467" t="n">

</xml_diff>

<commit_message>
subdivision of area 2 according to time class
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4752,7 +4752,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5176,7 +5176,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5580,7 +5580,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6104,7 +6104,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6524,7 +6524,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6628,7 +6628,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6736,7 +6736,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -6836,7 +6836,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -6936,7 +6936,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7044,7 +7044,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7144,7 +7144,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7248,7 +7248,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7656,7 +7656,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7764,7 +7764,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -7868,7 +7868,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -7976,7 +7976,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8172,7 +8172,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8272,7 +8272,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -8580,7 +8580,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8688,7 +8688,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -8892,7 +8892,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -8996,7 +8996,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9100,7 +9100,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9208,7 +9208,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9316,7 +9316,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9416,7 +9416,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -9516,7 +9516,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -9708,7 +9708,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -9812,7 +9812,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -9912,7 +9912,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10316,7 +10316,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -10424,7 +10424,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -10532,7 +10532,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -10632,7 +10632,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -10740,7 +10740,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -10848,7 +10848,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -10956,7 +10956,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11056,7 +11056,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11160,7 +11160,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11260,7 +11260,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -11364,7 +11364,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -11468,7 +11468,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -11576,7 +11576,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -11680,7 +11680,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -11780,7 +11780,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -11876,7 +11876,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -11980,7 +11980,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12080,7 +12080,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12184,7 +12184,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12292,7 +12292,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -12400,7 +12400,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -12504,7 +12504,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -12608,7 +12608,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -12712,7 +12712,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -12812,7 +12812,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13028,7 +13028,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13136,7 +13136,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13236,7 +13236,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -13336,7 +13336,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -13432,7 +13432,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -13536,7 +13536,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -13632,7 +13632,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -13848,7 +13848,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -13948,7 +13948,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14052,7 +14052,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14152,7 +14152,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -14248,7 +14248,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -14356,7 +14356,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -14456,7 +14456,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -14560,7 +14560,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -14664,7 +14664,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -14760,7 +14760,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -14868,7 +14868,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -14972,7 +14972,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -15180,7 +15180,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -15284,7 +15284,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -15384,7 +15384,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -15484,7 +15484,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -15584,7 +15584,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -15684,7 +15684,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -15784,7 +15784,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -15892,7 +15892,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16000,7 +16000,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -16212,7 +16212,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -16312,7 +16312,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -16416,7 +16416,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -16524,7 +16524,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -16628,7 +16628,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -16728,7 +16728,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -16824,7 +16824,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -16932,7 +16932,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -17036,7 +17036,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -17144,7 +17144,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -17252,7 +17252,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -17356,7 +17356,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -17456,7 +17456,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -17560,7 +17560,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -17660,7 +17660,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -17760,7 +17760,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -17860,7 +17860,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -17964,7 +17964,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -18172,7 +18172,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -18276,7 +18276,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -18384,7 +18384,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -18488,7 +18488,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -18592,7 +18592,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -18696,7 +18696,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -18796,7 +18796,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -18900,7 +18900,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -19004,7 +19004,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -19104,7 +19104,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -19208,7 +19208,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -19308,7 +19308,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -19408,7 +19408,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -19516,7 +19516,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -19620,7 +19620,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -19728,7 +19728,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -19832,7 +19832,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -19936,7 +19936,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -20036,7 +20036,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -20140,7 +20140,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -20248,7 +20248,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -20456,7 +20456,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -20560,7 +20560,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -20664,7 +20664,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -20760,7 +20760,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -20860,7 +20860,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -21072,7 +21072,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -21276,7 +21276,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -21376,7 +21376,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -21480,7 +21480,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -21576,7 +21576,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -21676,7 +21676,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -21776,7 +21776,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -21880,7 +21880,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -21980,7 +21980,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -22084,7 +22084,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -22288,7 +22288,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -22392,7 +22392,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -22492,7 +22492,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -22596,7 +22596,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -22700,7 +22700,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -22804,7 +22804,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -22912,7 +22912,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -23020,7 +23020,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -23128,7 +23128,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -23232,7 +23232,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -23332,7 +23332,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -23532,7 +23532,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -23636,7 +23636,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -23736,7 +23736,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -23836,7 +23836,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -23936,7 +23936,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -24036,7 +24036,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -24140,7 +24140,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -24236,7 +24236,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -24336,7 +24336,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -24440,7 +24440,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -24544,7 +24544,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -24640,7 +24640,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -24744,7 +24744,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -24844,7 +24844,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -24948,7 +24948,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -25048,7 +25048,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -25148,7 +25148,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -25248,7 +25248,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -25348,7 +25348,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -25456,7 +25456,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -25556,7 +25556,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -25660,7 +25660,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -25768,7 +25768,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -25872,7 +25872,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -25976,7 +25976,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -26080,7 +26080,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -26184,7 +26184,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -26284,7 +26284,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -26384,7 +26384,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -26484,7 +26484,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -26584,7 +26584,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -26684,7 +26684,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -26788,7 +26788,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -26896,7 +26896,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -27000,7 +27000,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -27100,7 +27100,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -27208,7 +27208,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -27308,7 +27308,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -27408,7 +27408,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -27516,7 +27516,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -27620,7 +27620,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -27716,7 +27716,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -27816,7 +27816,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -27916,7 +27916,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -28020,7 +28020,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -28120,7 +28120,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -28224,7 +28224,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -28332,7 +28332,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -28428,7 +28428,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -28532,7 +28532,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -28632,7 +28632,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -28736,7 +28736,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -28840,7 +28840,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -28944,7 +28944,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -29044,7 +29044,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -29152,7 +29152,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -29252,7 +29252,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -29356,7 +29356,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -29460,7 +29460,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -29556,7 +29556,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -29656,7 +29656,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -29760,7 +29760,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -29868,7 +29868,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -29968,7 +29968,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -30072,7 +30072,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -30180,7 +30180,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -30284,7 +30284,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -30388,7 +30388,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -30492,7 +30492,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -30592,7 +30592,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -30700,7 +30700,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -30808,7 +30808,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -30916,7 +30916,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -31020,7 +31020,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -31120,7 +31120,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -31224,7 +31224,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -31328,7 +31328,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -31436,7 +31436,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -31536,7 +31536,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -31632,7 +31632,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -31732,7 +31732,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -31836,7 +31836,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -31940,7 +31940,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -32044,7 +32044,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -32144,7 +32144,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -32244,7 +32244,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -32352,7 +32352,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -32452,7 +32452,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -32552,7 +32552,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -32660,7 +32660,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -32768,7 +32768,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -32868,7 +32868,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -32972,7 +32972,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -33080,7 +33080,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -33180,7 +33180,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -33280,7 +33280,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -33384,7 +33384,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -33484,7 +33484,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -33584,7 +33584,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -33684,7 +33684,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -33780,7 +33780,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -33884,7 +33884,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -33980,7 +33980,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -34088,7 +34088,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -34188,7 +34188,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -34288,7 +34288,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -34384,7 +34384,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -34492,7 +34492,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -34600,7 +34600,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -34700,7 +34700,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -34804,7 +34804,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -34900,7 +34900,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -35004,7 +35004,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -35104,7 +35104,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -35200,7 +35200,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -35304,7 +35304,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -35408,7 +35408,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -35512,7 +35512,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -35620,7 +35620,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -35720,7 +35720,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -35824,7 +35824,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -35924,7 +35924,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -36024,7 +36024,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -36132,7 +36132,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -36232,7 +36232,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -36328,7 +36328,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -36436,7 +36436,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -36540,7 +36540,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -36640,7 +36640,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -36748,7 +36748,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -36848,7 +36848,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -36952,7 +36952,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -37056,7 +37056,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -37152,7 +37152,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -37252,7 +37252,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -37360,7 +37360,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -37460,7 +37460,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -37564,7 +37564,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -37664,7 +37664,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -37764,7 +37764,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -37860,7 +37860,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -37956,7 +37956,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -38060,7 +38060,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -38160,7 +38160,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -38264,7 +38264,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -38360,7 +38360,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -38460,7 +38460,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -38560,7 +38560,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -38660,7 +38660,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -38756,7 +38756,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -38852,7 +38852,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -38952,7 +38952,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -39056,7 +39056,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -39156,7 +39156,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -39256,7 +39256,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -39360,7 +39360,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -39464,7 +39464,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -39560,7 +39560,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -39664,7 +39664,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -39760,7 +39760,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -39864,7 +39864,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -39964,7 +39964,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -40072,7 +40072,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -40172,7 +40172,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -40280,7 +40280,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -40380,7 +40380,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -40488,7 +40488,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -40592,7 +40592,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -40688,7 +40688,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -40788,7 +40788,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -40896,7 +40896,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -40996,7 +40996,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -41100,7 +41100,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -41196,7 +41196,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -41292,7 +41292,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -41392,7 +41392,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -41496,7 +41496,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -41596,7 +41596,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -41700,7 +41700,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -41800,7 +41800,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -41900,7 +41900,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -42004,7 +42004,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -42104,7 +42104,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -42200,7 +42200,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -42304,7 +42304,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -42404,7 +42404,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -42504,7 +42504,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -42608,7 +42608,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -42704,7 +42704,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -42804,7 +42804,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -42908,7 +42908,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -43016,7 +43016,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -43120,7 +43120,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -43224,7 +43224,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -43320,7 +43320,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -43416,7 +43416,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -43512,7 +43512,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -43616,7 +43616,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -43716,7 +43716,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -43820,7 +43820,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -43924,7 +43924,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -44032,7 +44032,7 @@
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
@@ -44132,7 +44132,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
@@ -44236,7 +44236,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -44336,7 +44336,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -44436,7 +44436,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -44536,7 +44536,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -44636,7 +44636,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
@@ -44736,7 +44736,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
@@ -44840,7 +44840,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -44948,7 +44948,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
@@ -45048,7 +45048,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
@@ -45148,7 +45148,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
@@ -45248,7 +45248,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -45348,7 +45348,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -45452,7 +45452,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -45556,7 +45556,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -45656,7 +45656,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -45756,7 +45756,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -45856,7 +45856,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -45960,7 +45960,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -46056,7 +46056,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -46152,7 +46152,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -46252,7 +46252,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -46348,7 +46348,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -46452,7 +46452,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -46552,7 +46552,7 @@
       </c>
       <c r="E451" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -46652,7 +46652,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -46748,7 +46748,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -46844,7 +46844,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
@@ -46940,7 +46940,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
@@ -47040,7 +47040,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -47136,7 +47136,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
@@ -47236,7 +47236,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
@@ -47340,7 +47340,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
@@ -47440,7 +47440,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -47548,7 +47548,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
@@ -47648,7 +47648,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -47748,7 +47748,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
@@ -47844,7 +47844,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
@@ -47944,7 +47944,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -48040,7 +48040,7 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
@@ -48144,7 +48144,7 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">

</xml_diff>

<commit_message>
first contourmaps cluster analysis
- contourmap for area1 is good
- othr groups something still wrong, look nto it after preprocessing of Mali and Fe-number
- Area 3b is finer area of 3a with little data points, so cluster analysis of this area won't say much
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area4.xlsx
+++ b/_INTERPOLATION/area4.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1656,7 +1656,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2072,7 +2072,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3004,7 +3004,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3404,7 +3404,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4132,7 +4132,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4340,7 +4340,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4648,7 +4648,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4752,7 +4752,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5176,7 +5176,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5380,7 +5380,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5580,7 +5580,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5688,7 +5688,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5788,7 +5788,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -5896,7 +5896,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6104,7 +6104,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6524,7 +6524,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6628,7 +6628,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6736,7 +6736,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -6836,7 +6836,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -6936,7 +6936,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7044,7 +7044,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7144,7 +7144,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7248,7 +7248,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7656,7 +7656,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7764,7 +7764,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -7868,7 +7868,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -7976,7 +7976,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8172,7 +8172,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8272,7 +8272,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -8580,7 +8580,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8688,7 +8688,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -8788,7 +8788,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -8892,7 +8892,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -8996,7 +8996,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9100,7 +9100,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9208,7 +9208,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9316,7 +9316,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9416,7 +9416,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -9516,7 +9516,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -9612,7 +9612,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -9708,7 +9708,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -9812,7 +9812,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -9912,7 +9912,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10012,7 +10012,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10112,7 +10112,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10316,7 +10316,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -10424,7 +10424,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -10532,7 +10532,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -10632,7 +10632,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -10740,7 +10740,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -10848,7 +10848,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -10956,7 +10956,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11056,7 +11056,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11160,7 +11160,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11260,7 +11260,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -11364,7 +11364,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -11468,7 +11468,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -11576,7 +11576,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -11680,7 +11680,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -11780,7 +11780,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -11876,7 +11876,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -11980,7 +11980,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12080,7 +12080,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12184,7 +12184,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12292,7 +12292,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -12400,7 +12400,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -12504,7 +12504,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -12608,7 +12608,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -12712,7 +12712,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -12812,7 +12812,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13028,7 +13028,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13136,7 +13136,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13236,7 +13236,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -13336,7 +13336,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -13432,7 +13432,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -13536,7 +13536,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -13632,7 +13632,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -13740,7 +13740,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -13848,7 +13848,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -13948,7 +13948,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14052,7 +14052,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14152,7 +14152,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -14248,7 +14248,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -14356,7 +14356,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -14456,7 +14456,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -14560,7 +14560,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -14664,7 +14664,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -14760,7 +14760,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -14868,7 +14868,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -14972,7 +14972,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -15180,7 +15180,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -15284,7 +15284,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -15384,7 +15384,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -15484,7 +15484,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -15584,7 +15584,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -15684,7 +15684,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -15784,7 +15784,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -15892,7 +15892,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16000,7 +16000,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -16108,7 +16108,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -16212,7 +16212,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -16312,7 +16312,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -16416,7 +16416,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -16524,7 +16524,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -16628,7 +16628,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -16728,7 +16728,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -16824,7 +16824,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -16932,7 +16932,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -17036,7 +17036,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -17144,7 +17144,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -17252,7 +17252,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -17356,7 +17356,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -17456,7 +17456,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -17560,7 +17560,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -17660,7 +17660,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -17760,7 +17760,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -17860,7 +17860,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -17964,7 +17964,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -18072,7 +18072,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -18172,7 +18172,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -18276,7 +18276,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -18384,7 +18384,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -18488,7 +18488,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -18592,7 +18592,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -18696,7 +18696,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -18796,7 +18796,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -18900,7 +18900,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -19004,7 +19004,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -19104,7 +19104,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -19208,7 +19208,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -19308,7 +19308,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -19408,7 +19408,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -19516,7 +19516,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -19620,7 +19620,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -19728,7 +19728,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -19832,7 +19832,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -19936,7 +19936,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -20036,7 +20036,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -20140,7 +20140,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -20248,7 +20248,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -20352,7 +20352,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -20456,7 +20456,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -20560,7 +20560,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -20664,7 +20664,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -20760,7 +20760,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -20860,7 +20860,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -20968,7 +20968,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -21072,7 +21072,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -21176,7 +21176,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -21276,7 +21276,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -21376,7 +21376,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -21480,7 +21480,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -21576,7 +21576,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -21676,7 +21676,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -21776,7 +21776,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -21880,7 +21880,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -21980,7 +21980,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -22084,7 +22084,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -22288,7 +22288,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -22392,7 +22392,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -22492,7 +22492,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -22596,7 +22596,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -22700,7 +22700,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -22804,7 +22804,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -22912,7 +22912,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -23020,7 +23020,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -23128,7 +23128,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -23232,7 +23232,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -23332,7 +23332,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -23532,7 +23532,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -23636,7 +23636,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -23736,7 +23736,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -23836,7 +23836,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -23936,7 +23936,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -24036,7 +24036,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -24140,7 +24140,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -24236,7 +24236,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -24336,7 +24336,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -24440,7 +24440,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -24544,7 +24544,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -24640,7 +24640,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -24744,7 +24744,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -24844,7 +24844,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -24948,7 +24948,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -25048,7 +25048,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -25148,7 +25148,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -25248,7 +25248,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -25348,7 +25348,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -25456,7 +25456,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -25556,7 +25556,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -25660,7 +25660,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -25768,7 +25768,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -25872,7 +25872,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -25976,7 +25976,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -26080,7 +26080,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -26184,7 +26184,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -26284,7 +26284,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -26384,7 +26384,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -26484,7 +26484,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -26584,7 +26584,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -26684,7 +26684,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -26788,7 +26788,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -26896,7 +26896,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -27000,7 +27000,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -27100,7 +27100,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -27208,7 +27208,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -27308,7 +27308,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -27408,7 +27408,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -27516,7 +27516,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -27620,7 +27620,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -27716,7 +27716,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -27816,7 +27816,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -27916,7 +27916,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -28020,7 +28020,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -28120,7 +28120,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -28224,7 +28224,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -28332,7 +28332,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -28428,7 +28428,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -28532,7 +28532,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -28632,7 +28632,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -28736,7 +28736,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -28840,7 +28840,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -28944,7 +28944,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -29044,7 +29044,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -29152,7 +29152,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -29252,7 +29252,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -29356,7 +29356,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -29460,7 +29460,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -29556,7 +29556,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -29656,7 +29656,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -29760,7 +29760,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -29868,7 +29868,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -29968,7 +29968,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -30072,7 +30072,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -30180,7 +30180,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -30284,7 +30284,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -30388,7 +30388,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -30492,7 +30492,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -30592,7 +30592,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -30700,7 +30700,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -30808,7 +30808,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -30916,7 +30916,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -31020,7 +31020,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -31120,7 +31120,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -31224,7 +31224,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -31328,7 +31328,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -31436,7 +31436,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -31536,7 +31536,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -31632,7 +31632,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -31732,7 +31732,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -31836,7 +31836,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -31940,7 +31940,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -32044,7 +32044,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -32144,7 +32144,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -32244,7 +32244,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -32352,7 +32352,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -32452,7 +32452,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -32552,7 +32552,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -32660,7 +32660,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -32768,7 +32768,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -32868,7 +32868,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -32972,7 +32972,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -33080,7 +33080,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -33180,7 +33180,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -33280,7 +33280,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -33384,7 +33384,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -33484,7 +33484,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -33584,7 +33584,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -33684,7 +33684,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -33780,7 +33780,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -33884,7 +33884,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -33980,7 +33980,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -34088,7 +34088,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -34188,7 +34188,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -34288,7 +34288,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -34384,7 +34384,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -34492,7 +34492,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -34600,7 +34600,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -34700,7 +34700,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -34804,7 +34804,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -34900,7 +34900,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -35004,7 +35004,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -35104,7 +35104,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -35200,7 +35200,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -35304,7 +35304,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -35408,7 +35408,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -35512,7 +35512,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -35620,7 +35620,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -35720,7 +35720,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -35824,7 +35824,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -35924,7 +35924,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -36024,7 +36024,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -36132,7 +36132,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -36232,7 +36232,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -36328,7 +36328,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -36436,7 +36436,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -36540,7 +36540,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -36640,7 +36640,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -36748,7 +36748,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -36848,7 +36848,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -36952,7 +36952,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -37056,7 +37056,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -37152,7 +37152,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -37252,7 +37252,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -37360,7 +37360,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -37460,7 +37460,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -37564,7 +37564,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -37664,7 +37664,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -37764,7 +37764,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -37860,7 +37860,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -37956,7 +37956,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -38060,7 +38060,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -38160,7 +38160,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -38264,7 +38264,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -38360,7 +38360,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -38460,7 +38460,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -38560,7 +38560,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -38660,7 +38660,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -38756,7 +38756,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -38852,7 +38852,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -38952,7 +38952,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -39056,7 +39056,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -39156,7 +39156,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -39256,7 +39256,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -39360,7 +39360,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -39464,7 +39464,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -39560,7 +39560,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -39664,7 +39664,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -39760,7 +39760,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -39864,7 +39864,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -39964,7 +39964,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -40072,7 +40072,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -40172,7 +40172,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -40280,7 +40280,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -40380,7 +40380,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -40488,7 +40488,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -40592,7 +40592,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -40688,7 +40688,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -40788,7 +40788,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -40896,7 +40896,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -40996,7 +40996,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -41100,7 +41100,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -41196,7 +41196,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -41292,7 +41292,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -41392,7 +41392,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -41496,7 +41496,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -41596,7 +41596,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -41700,7 +41700,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -41800,7 +41800,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -41900,7 +41900,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -42004,7 +42004,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -42104,7 +42104,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -42200,7 +42200,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -42304,7 +42304,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -42404,7 +42404,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -42504,7 +42504,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -42608,7 +42608,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -42704,7 +42704,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -42804,7 +42804,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -42908,7 +42908,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -43016,7 +43016,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -43120,7 +43120,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -43224,7 +43224,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -43320,7 +43320,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -43416,7 +43416,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -43512,7 +43512,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -43616,7 +43616,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -43716,7 +43716,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -43820,7 +43820,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -43924,7 +43924,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -44032,7 +44032,7 @@
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
@@ -44132,7 +44132,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
@@ -44236,7 +44236,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -44336,7 +44336,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -44436,7 +44436,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -44536,7 +44536,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -44636,7 +44636,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
@@ -44736,7 +44736,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
@@ -44840,7 +44840,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -44948,7 +44948,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
@@ -45048,7 +45048,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
@@ -45148,7 +45148,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
@@ -45248,7 +45248,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -45348,7 +45348,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -45452,7 +45452,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -45556,7 +45556,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -45656,7 +45656,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -45756,7 +45756,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -45856,7 +45856,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -45960,7 +45960,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -46056,7 +46056,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -46152,7 +46152,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -46252,7 +46252,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -46348,7 +46348,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -46452,7 +46452,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -46552,7 +46552,7 @@
       </c>
       <c r="E451" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -46652,7 +46652,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -46748,7 +46748,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -46844,7 +46844,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
@@ -46940,7 +46940,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
@@ -47040,7 +47040,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -47136,7 +47136,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
@@ -47236,7 +47236,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
@@ -47340,7 +47340,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
@@ -47440,7 +47440,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -47548,7 +47548,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
@@ -47648,7 +47648,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -47748,7 +47748,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
@@ -47844,7 +47844,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
@@ -47944,7 +47944,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -48040,7 +48040,7 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
@@ -48144,7 +48144,7 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">

</xml_diff>